<commit_message>
update and reorg to include 2015 and 2016
Fixed some things in the core forge and IN methods to correct a location issue for state-specific data. I also moved around some of the functions in the predict function and reconciled an issue in loadLearnedMaterials related to the state-specific reorg. I uploaded the 2015 and 2016 datasets for Indiana and did a full recompile for all plots and charts.
</commit_message>
<xml_diff>
--- a/data/IN/outputs/583138/t_set_test.xlsx
+++ b/data/IN/outputs/583138/t_set_test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1031,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="U62" sqref="U62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:Q102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,31 +1101,31 @@
         <v>12</v>
       </c>
       <c r="H2">
-        <v>0.88871722273924258</v>
+        <v>0.82334695044007744</v>
       </c>
       <c r="I2">
-        <v>0.82025687537040537</v>
+        <v>0.74148136071386206</v>
       </c>
       <c r="J2">
-        <v>0.70823288298036635</v>
+        <v>0.63175111320469401</v>
       </c>
       <c r="K2">
-        <v>0.51150643096657278</v>
+        <v>0.24233767590600763</v>
       </c>
       <c r="L2">
-        <v>0.39046127486871351</v>
+        <v>0.19992458475738231</v>
       </c>
       <c r="M2">
-        <v>0.22238013666901799</v>
+        <v>0.11427933743806241</v>
       </c>
       <c r="N2">
-        <v>9.6359593389283973E-2</v>
+        <v>8.5682739118865744E-2</v>
       </c>
       <c r="O2">
-        <v>6.4720618386268608E-2</v>
+        <v>4.8122454388870167E-2</v>
       </c>
       <c r="P2">
-        <v>4.4098438323569113E-2</v>
+        <v>2.0180944579190913E-2</v>
       </c>
       <c r="Q2">
         <v>1</v>
@@ -1142,31 +1142,31 @@
         <v>14</v>
       </c>
       <c r="H3">
-        <v>0.89010944492407706</v>
+        <v>0.78599878599346451</v>
       </c>
       <c r="I3">
-        <v>0.82553052429729423</v>
+        <v>0.76320888443852264</v>
       </c>
       <c r="J3">
-        <v>0.72108649356819265</v>
+        <v>0.66442092522192708</v>
       </c>
       <c r="K3">
-        <v>0.51858858764311055</v>
+        <v>0.26151992399204282</v>
       </c>
       <c r="L3">
-        <v>0.35960341505454635</v>
+        <v>0.25139360568123936</v>
       </c>
       <c r="M3">
-        <v>0.15567907150150465</v>
+        <v>0.13964492772554285</v>
       </c>
       <c r="N3">
-        <v>5.0733157734197967E-2</v>
+        <v>0.10693353031892805</v>
       </c>
       <c r="O3">
-        <v>3.2706018832267099E-2</v>
+        <v>6.0418353230046982E-2</v>
       </c>
       <c r="P3">
-        <v>2.473173325761991E-2</v>
+        <v>2.8094919585329104E-2</v>
       </c>
       <c r="Q3">
         <v>1</v>
@@ -1183,31 +1183,31 @@
         <v>16</v>
       </c>
       <c r="H4">
-        <v>1.2299219553580763E-2</v>
+        <v>2.9582972721955873E-2</v>
       </c>
       <c r="I4">
-        <v>4.5077244237221661E-3</v>
+        <v>2.2061084252196217E-2</v>
       </c>
       <c r="J4">
-        <v>1.5500972440688388E-3</v>
+        <v>8.7350403165519855E-3</v>
       </c>
       <c r="K4">
-        <v>5.3655904990527776E-4</v>
+        <v>1.8063411649905505E-3</v>
       </c>
       <c r="L4">
-        <v>1.7712816308040056E-4</v>
+        <v>9.1929476591679903E-4</v>
       </c>
       <c r="M4">
-        <v>7.381102779036463E-5</v>
+        <v>2.9268633348336333E-4</v>
       </c>
       <c r="N4">
-        <v>2.6192257136851585E-5</v>
+        <v>1.6650314803831579E-4</v>
       </c>
       <c r="O4">
-        <v>1.0526025249604262E-5</v>
+        <v>6.1562170066844523E-5</v>
       </c>
       <c r="P4">
-        <v>4.6114288127880679E-6</v>
+        <v>2.8648685461435711E-5</v>
       </c>
       <c r="Q4">
         <v>1</v>
@@ -1224,28 +1224,28 @@
         <v>18</v>
       </c>
       <c r="H5">
-        <v>0.99999999999879963</v>
+        <v>0.99999999999842881</v>
       </c>
       <c r="I5">
-        <v>0.99999999999978717</v>
+        <v>0.9999999999996485</v>
       </c>
       <c r="J5">
-        <v>0.99999999999996314</v>
+        <v>0.99999999999995048</v>
       </c>
       <c r="K5">
-        <v>0.99999999999999167</v>
+        <v>0.99999999999996836</v>
       </c>
       <c r="L5">
-        <v>0.999999999999999</v>
+        <v>0.99999999999999478</v>
       </c>
       <c r="M5">
-        <v>0.999999999999999</v>
+        <v>0.99999999999999911</v>
       </c>
       <c r="N5">
-        <v>0.99999999999999911</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="O5">
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="P5">
         <v>1</v>
@@ -1265,31 +1265,31 @@
         <v>20</v>
       </c>
       <c r="H6">
-        <v>0.99999999984252463</v>
+        <v>0.99999999995276079</v>
       </c>
       <c r="I6">
-        <v>0.99999999996259969</v>
+        <v>0.99999999998551325</v>
       </c>
       <c r="J6">
-        <v>0.99999999999368572</v>
+        <v>0.99</v>
       </c>
       <c r="K6">
-        <v>0.99999999999904554</v>
+        <v>0.99472903969691984</v>
       </c>
       <c r="L6">
-        <v>0.99999999999991085</v>
+        <v>0.9990961290921343</v>
       </c>
       <c r="M6">
-        <v>0.99999999999993783</v>
+        <v>0.99985114934734975</v>
       </c>
       <c r="N6">
-        <v>0.99999999999996214</v>
+        <v>0.99997118673749275</v>
       </c>
       <c r="O6">
-        <v>0.99999999999999323</v>
+        <v>0.99999635265979225</v>
       </c>
       <c r="P6">
-        <v>0.99999999999999833</v>
+        <v>0.99999737647190134</v>
       </c>
       <c r="Q6">
         <v>1</v>
@@ -1306,31 +1306,31 @@
         <v>22</v>
       </c>
       <c r="H7">
-        <v>7.4900128877275318E-2</v>
+        <v>0.3120689772044794</v>
       </c>
       <c r="I7">
-        <v>4.0400550092324565E-2</v>
+        <v>0.29408579986318861</v>
       </c>
       <c r="J7">
-        <v>1.9353130065499845E-2</v>
+        <v>0.18581749873045644</v>
       </c>
       <c r="K7">
-        <v>7.9421513067220988E-3</v>
+        <v>5.6356872073293277E-2</v>
       </c>
       <c r="L7">
-        <v>3.6414827743594278E-3</v>
+        <v>3.5604943614427807E-2</v>
       </c>
       <c r="M7">
-        <v>1.7942135206110907E-3</v>
+        <v>1.9086182249472085E-2</v>
       </c>
       <c r="N7">
-        <v>7.1845884939338684E-4</v>
+        <v>1.237996928524431E-2</v>
       </c>
       <c r="O7">
-        <v>3.5580177767718073E-4</v>
+        <v>6.143740948846497E-3</v>
       </c>
       <c r="P7">
-        <v>2.0177436105826615E-4</v>
+        <v>2.8128503332739228E-3</v>
       </c>
       <c r="Q7">
         <v>1</v>
@@ -1346,44 +1346,41 @@
       <c r="C8" t="s">
         <v>24</v>
       </c>
-      <c r="D8">
-        <v>0.5</v>
-      </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0.76</v>
       </c>
       <c r="G8">
-        <v>0.01</v>
+        <v>0.24</v>
       </c>
       <c r="H8">
-        <v>0.01</v>
+        <v>0.24</v>
       </c>
       <c r="I8">
-        <v>8.599107434418201E-3</v>
+        <v>0.22168674698795177</v>
       </c>
       <c r="J8">
-        <v>8.2871130810506476E-3</v>
+        <v>0.22349874737454758</v>
       </c>
       <c r="K8">
-        <v>4.8914637413294271E-3</v>
+        <v>9.4558138794004529E-2</v>
       </c>
       <c r="L8">
-        <v>4.187225368279251E-3</v>
+        <v>9.9137915247995714E-2</v>
       </c>
       <c r="M8">
-        <v>1.2081478036263971E-3</v>
+        <v>8.6005817008786428E-2</v>
       </c>
       <c r="N8">
-        <v>3.0634045498107999E-4</v>
+        <v>9.4952865085770291E-2</v>
       </c>
       <c r="O8">
-        <v>3.099433432963303E-4</v>
+        <v>8.500460929712389E-2</v>
       </c>
       <c r="P8">
-        <v>2.7589303207791528E-4</v>
+        <v>2.188797284000308E-2</v>
       </c>
       <c r="Q8">
         <v>1</v>
@@ -1400,31 +1397,31 @@
         <v>26</v>
       </c>
       <c r="H9">
-        <v>0.11357404378582359</v>
+        <v>0.12026048398063965</v>
       </c>
       <c r="I9">
-        <v>6.3397768876622379E-2</v>
+        <v>9.6104275697837693E-2</v>
       </c>
       <c r="J9">
-        <v>3.0294686300111059E-2</v>
+        <v>4.8152841731477256E-2</v>
       </c>
       <c r="K9">
-        <v>1.3252769799341169E-2</v>
+        <v>1.4736293621224254E-2</v>
       </c>
       <c r="L9">
-        <v>6.3358229813028823E-3</v>
+        <v>9.3924253406245679E-3</v>
       </c>
       <c r="M9">
-        <v>1.3231760475673478E-3</v>
+        <v>4.987502000284757E-3</v>
       </c>
       <c r="N9">
-        <v>2.3474245607129379E-4</v>
+        <v>3.2992218447144262E-3</v>
       </c>
       <c r="O9">
-        <v>1.2744529527144598E-4</v>
+        <v>1.6204077476434041E-3</v>
       </c>
       <c r="P9">
-        <v>8.0294322280447271E-5</v>
+        <v>5.2285434389198965E-4</v>
       </c>
       <c r="Q9">
         <v>1</v>
@@ -1441,31 +1438,31 @@
         <v>28</v>
       </c>
       <c r="H10">
-        <v>0.43353497163614502</v>
+        <v>0.5489627975150162</v>
       </c>
       <c r="I10">
-        <v>0.27855886415836212</v>
+        <v>0.460658748411852</v>
       </c>
       <c r="J10">
-        <v>0.18447799302362514</v>
+        <v>0.27780999849572213</v>
       </c>
       <c r="K10">
-        <v>9.6511271965940934E-2</v>
+        <v>9.3745336439588087E-2</v>
       </c>
       <c r="L10">
-        <v>5.824167454524494E-2</v>
+        <v>6.0628102940472363E-2</v>
       </c>
       <c r="M10">
-        <v>2.8172466106711976E-2</v>
+        <v>3.3671036116852369E-2</v>
       </c>
       <c r="N10">
-        <v>8.7800278641471819E-3</v>
+        <v>2.161141420838153E-2</v>
       </c>
       <c r="O10">
-        <v>6.1979597156866196E-3</v>
+        <v>1.2030651146664802E-2</v>
       </c>
       <c r="P10">
-        <v>4.1201142100547898E-3</v>
+        <v>4.2736042988590559E-3</v>
       </c>
       <c r="Q10">
         <v>1</v>
@@ -1482,31 +1479,31 @@
         <v>30</v>
       </c>
       <c r="H11">
-        <v>0.93608310127873706</v>
+        <v>0.90228763247918653</v>
       </c>
       <c r="I11">
-        <v>0.90847744927289953</v>
+        <v>0.90003264988773624</v>
       </c>
       <c r="J11">
-        <v>0.87399874476713557</v>
+        <v>0.83061081285917282</v>
       </c>
       <c r="K11">
-        <v>0.80030810301676081</v>
+        <v>0.6110530859717398</v>
       </c>
       <c r="L11">
-        <v>0.74455267685019899</v>
+        <v>0.54593550719822437</v>
       </c>
       <c r="M11">
-        <v>0.53829402515871205</v>
+        <v>0.4344388772131364</v>
       </c>
       <c r="N11">
-        <v>0.27637245760949553</v>
+        <v>0.35902094201558465</v>
       </c>
       <c r="O11">
-        <v>0.24815413175961212</v>
+        <v>0.26898323886227149</v>
       </c>
       <c r="P11">
-        <v>0.20645300989962859</v>
+        <v>9.7350453700788916E-2</v>
       </c>
       <c r="Q11">
         <v>1</v>
@@ -1526,28 +1523,28 @@
         <v>0.99999981069727872</v>
       </c>
       <c r="I12">
-        <v>0.99999993067786841</v>
+        <v>0.99</v>
       </c>
       <c r="J12">
-        <v>0.99999997689262177</v>
+        <v>0.99691192266380235</v>
       </c>
       <c r="K12">
-        <v>0.99999999108715398</v>
+        <v>0.99757636428298591</v>
       </c>
       <c r="L12">
-        <v>0.99999999640358839</v>
+        <v>0.9993774329598496</v>
       </c>
       <c r="M12">
-        <v>0.99999999502035308</v>
+        <v>0.99975629445722214</v>
       </c>
       <c r="N12">
-        <v>0.99999999512630289</v>
+        <v>0.99994799951493296</v>
       </c>
       <c r="O12">
-        <v>0.99999999839768861</v>
+        <v>0.99998239923035137</v>
       </c>
       <c r="P12">
-        <v>0.999999999563006</v>
+        <v>0.99998086875792314</v>
       </c>
       <c r="Q12">
         <v>1</v>
@@ -1579,28 +1576,28 @@
         <v>0.01</v>
       </c>
       <c r="I13">
-        <v>5.5248618784530393E-3</v>
+        <v>7.8600903910394978E-3</v>
       </c>
       <c r="J13">
-        <v>2.9154518950437322E-3</v>
+        <v>4.1387917961386378E-3</v>
       </c>
       <c r="K13">
-        <v>1.1682242990654205E-3</v>
+        <v>0.01</v>
       </c>
       <c r="L13">
-        <v>5.537098560354373E-4</v>
+        <v>8.249852681202121E-3</v>
       </c>
       <c r="M13">
-        <v>2.1979954281695083E-4</v>
+        <v>3.9833382650854713E-3</v>
       </c>
       <c r="N13">
-        <v>6.7889584379964395E-5</v>
+        <v>3.0107638877587225E-3</v>
       </c>
       <c r="O13">
-        <v>4.4057056922150873E-5</v>
+        <v>1.4316165273780895E-3</v>
       </c>
       <c r="P13">
-        <v>3.0648798383712991E-5</v>
+        <v>7.813902200031796E-4</v>
       </c>
       <c r="Q13">
         <v>1</v>
@@ -1616,9 +1613,6 @@
       <c r="C14" t="s">
         <v>36</v>
       </c>
-      <c r="D14">
-        <v>0.5</v>
-      </c>
       <c r="E14">
         <v>1</v>
       </c>
@@ -1632,28 +1626,28 @@
         <v>0.99</v>
       </c>
       <c r="I14">
-        <v>0.99776035834266519</v>
+        <v>0.99741668819426499</v>
       </c>
       <c r="J14">
-        <v>0.99962117348797219</v>
+        <v>0.99966493550008373</v>
       </c>
       <c r="K14">
-        <v>0.99991579151923438</v>
+        <v>0.9997977790360415</v>
       </c>
       <c r="L14">
-        <v>0.99998695268718185</v>
+        <v>0.99996254550186459</v>
       </c>
       <c r="M14">
-        <v>0.99998825740314268</v>
+        <v>0.99999088918816303</v>
       </c>
       <c r="N14">
-        <v>0.99998986911579479</v>
+        <v>0.99999877031018336</v>
       </c>
       <c r="O14">
-        <v>0.99999910936458747</v>
+        <v>0.99999985305577466</v>
       </c>
       <c r="P14">
-        <v>0.99999976324865958</v>
+        <v>0.99999988026766506</v>
       </c>
       <c r="Q14">
         <v>1</v>
@@ -1670,31 +1664,31 @@
         <v>38</v>
       </c>
       <c r="H15">
-        <v>7.5709029901932054E-2</v>
+        <v>0.19296363819016454</v>
       </c>
       <c r="I15">
-        <v>3.3913921439308228E-2</v>
+        <v>0.13398376396534098</v>
       </c>
       <c r="J15">
-        <v>1.4329876286168452E-2</v>
+        <v>6.1391580957416439E-2</v>
       </c>
       <c r="K15">
-        <v>5.7247443467378064E-3</v>
+        <v>1.3466343236242755E-2</v>
       </c>
       <c r="L15">
-        <v>2.559366913052751E-3</v>
+        <v>6.3826058316338759E-3</v>
       </c>
       <c r="M15">
-        <v>1.1441956023873199E-3</v>
+        <v>2.767949056611652E-3</v>
       </c>
       <c r="N15">
-        <v>4.0076652177523157E-4</v>
+        <v>1.7485495605029304E-3</v>
       </c>
       <c r="O15">
-        <v>1.9843942584716882E-4</v>
+        <v>7.3641614259962627E-4</v>
       </c>
       <c r="P15">
-        <v>1.0121394875261641E-4</v>
+        <v>2.9886565820735667E-4</v>
       </c>
       <c r="Q15">
         <v>1</v>
@@ -1710,44 +1704,41 @@
       <c r="C16" t="s">
         <v>40</v>
       </c>
-      <c r="D16">
-        <v>0.5</v>
-      </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="G16">
+        <v>0.1333333333333333</v>
+      </c>
+      <c r="H16">
+        <v>0.1333333333333333</v>
+      </c>
+      <c r="I16">
+        <v>0.41899441340782112</v>
+      </c>
+      <c r="J16">
+        <v>0.7884028484231943</v>
+      </c>
+      <c r="K16">
+        <v>0.83149044251275428</v>
+      </c>
+      <c r="L16">
+        <v>0.9578558048829704</v>
+      </c>
+      <c r="M16">
+        <v>0.98964712724240234</v>
+      </c>
+      <c r="N16">
         <v>0.99</v>
       </c>
-      <c r="H16">
-        <v>0.99</v>
-      </c>
-      <c r="I16">
-        <v>0.99787798408488071</v>
-      </c>
-      <c r="J16">
-        <v>0.99960522919481942</v>
-      </c>
-      <c r="K16">
-        <v>0.99989722142063708</v>
-      </c>
-      <c r="L16">
-        <v>0.99998772682001968</v>
-      </c>
-      <c r="M16">
-        <v>0.99998772682001968</v>
-      </c>
-      <c r="N16">
-        <v>0.9999892935921787</v>
-      </c>
       <c r="O16">
-        <v>0.99999869432823529</v>
+        <v>0.99819205896669205</v>
       </c>
       <c r="P16">
-        <v>0.9999996866384655</v>
+        <v>0.99858145387338104</v>
       </c>
       <c r="Q16">
         <v>1</v>
@@ -1764,28 +1755,28 @@
         <v>42</v>
       </c>
       <c r="H17">
-        <v>0.99999999998610556</v>
+        <v>0.99999999999421263</v>
       </c>
       <c r="I17">
-        <v>0.99999999999818379</v>
+        <v>0.9999999999982252</v>
       </c>
       <c r="J17">
-        <v>0.99999999999973133</v>
+        <v>0.99999999999979439</v>
       </c>
       <c r="K17">
-        <v>0.99999999999994937</v>
+        <v>0.99999999999989719</v>
       </c>
       <c r="L17">
-        <v>0.99999999999999456</v>
+        <v>0.99999999999998057</v>
       </c>
       <c r="M17">
-        <v>0.99999999999999512</v>
+        <v>0.99999999999999722</v>
       </c>
       <c r="N17">
-        <v>0.99999999999999656</v>
+        <v>0.99999999999999967</v>
       </c>
       <c r="O17">
-        <v>0.99999999999999967</v>
+        <v>1</v>
       </c>
       <c r="P17">
         <v>1</v>
@@ -1805,31 +1796,31 @@
         <v>44</v>
       </c>
       <c r="H18">
-        <v>0.99999980731396398</v>
+        <v>0.99999987937970847</v>
       </c>
       <c r="I18">
-        <v>0.99999992774272783</v>
+        <v>0.99999995869167779</v>
       </c>
       <c r="J18">
-        <v>0.99999998317296312</v>
+        <v>0.99999999225468938</v>
       </c>
       <c r="K18">
-        <v>0.9999999954696438</v>
+        <v>0.99999999593688627</v>
       </c>
       <c r="L18">
-        <v>0.99999999914645454</v>
+        <v>0.99999999898422154</v>
       </c>
       <c r="M18">
-        <v>0.99999999929418359</v>
+        <v>0.9999999997780088</v>
       </c>
       <c r="N18">
-        <v>0.99999999962432351</v>
+        <v>0.99999999993590394</v>
       </c>
       <c r="O18">
-        <v>0.99999999988630839</v>
+        <v>0.99999999998235034</v>
       </c>
       <c r="P18">
-        <v>0.99999999997157707</v>
+        <v>0.99999999998561884</v>
       </c>
       <c r="Q18">
         <v>0</v>
@@ -1846,31 +1837,31 @@
         <v>46</v>
       </c>
       <c r="H19">
-        <v>0.99999999932632855</v>
+        <v>0.99999999770399639</v>
       </c>
       <c r="I19">
-        <v>0.99999999989088417</v>
+        <v>0.99999999908159853</v>
       </c>
       <c r="J19">
-        <v>0.99999999998916578</v>
+        <v>0.99999999979764043</v>
       </c>
       <c r="K19">
-        <v>0.9999999999974204</v>
+        <v>0.99999999988710464</v>
       </c>
       <c r="L19">
-        <v>0.99999999999967271</v>
+        <v>0.99999999997394728</v>
       </c>
       <c r="M19">
-        <v>0.99999999999961686</v>
+        <v>0.99999999999565792</v>
       </c>
       <c r="N19">
-        <v>0.99999999999968725</v>
+        <v>0.99999999999873013</v>
       </c>
       <c r="O19">
-        <v>0.99999999999994671</v>
+        <v>0.99999999999976708</v>
       </c>
       <c r="P19">
-        <v>0.99999999999999134</v>
+        <v>0.99999999999978095</v>
       </c>
       <c r="Q19">
         <v>1</v>
@@ -1890,28 +1881,28 @@
         <v>0.7775198528860211</v>
       </c>
       <c r="I20">
-        <v>0.67321144144451739</v>
+        <v>0.7647590745304006</v>
       </c>
       <c r="J20">
-        <v>0.55371718757435395</v>
+        <v>0.6511172444362362</v>
       </c>
       <c r="K20">
-        <v>0.40959144657961233</v>
+        <v>0.32205975380240676</v>
       </c>
       <c r="L20">
-        <v>0.31892919419321014</v>
+        <v>0.2871222624885118</v>
       </c>
       <c r="M20">
-        <v>0.13501696622470891</v>
+        <v>0.19351271757913013</v>
       </c>
       <c r="N20">
-        <v>4.0417678634429945E-2</v>
+        <v>0.16339288186251064</v>
       </c>
       <c r="O20">
-        <v>2.8952116458176504E-2</v>
+        <v>0.10899916070039339</v>
       </c>
       <c r="P20">
-        <v>2.0126073424585635E-2</v>
+        <v>4.8763719476646948E-2</v>
       </c>
       <c r="Q20">
         <v>0</v>
@@ -1928,31 +1919,31 @@
         <v>50</v>
       </c>
       <c r="H21">
-        <v>0.99999999994565814</v>
+        <v>0.99999999943292972</v>
       </c>
       <c r="I21">
-        <v>0.99999999999025591</v>
+        <v>0.99999999979522458</v>
       </c>
       <c r="J21">
-        <v>0.99999999999820888</v>
+        <v>0.99999999994711097</v>
       </c>
       <c r="K21">
-        <v>0.99999999999950628</v>
+        <v>0.99999999996033317</v>
       </c>
       <c r="L21">
-        <v>0.9999999999999043</v>
+        <v>0.99999999998975486</v>
       </c>
       <c r="M21">
-        <v>0.99999999999989808</v>
+        <v>0.99999999999729861</v>
       </c>
       <c r="N21">
-        <v>0.99999999999989586</v>
+        <v>0.999999999999449</v>
       </c>
       <c r="O21">
-        <v>0.99999999999998612</v>
+        <v>0.99999999999985867</v>
       </c>
       <c r="P21">
-        <v>0.99999999999999667</v>
+        <v>0.99999999999983902</v>
       </c>
       <c r="Q21">
         <v>1</v>
@@ -1969,31 +1960,31 @@
         <v>52</v>
       </c>
       <c r="H22">
-        <v>0.999999994595687</v>
+        <v>0.9999999939306341</v>
       </c>
       <c r="I22">
-        <v>0.99999999879472157</v>
+        <v>0.99999999800459205</v>
       </c>
       <c r="J22">
-        <v>0.99999999975531939</v>
+        <v>0.99999999969766551</v>
       </c>
       <c r="K22">
-        <v>0.999999999971114</v>
+        <v>0.99999999987002441</v>
       </c>
       <c r="L22">
-        <v>0.99999999999638922</v>
+        <v>0.99999999996643008</v>
       </c>
       <c r="M22">
-        <v>0.99999999999732525</v>
+        <v>0.99999999999550404</v>
       </c>
       <c r="N22">
-        <v>0.99999999999848432</v>
+        <v>0.99999999999878242</v>
       </c>
       <c r="O22">
-        <v>0.99999999999967526</v>
+        <v>0.99999999999979039</v>
       </c>
       <c r="P22">
-        <v>0.99999999999994171</v>
+        <v>0.99999999999982037</v>
       </c>
       <c r="Q22">
         <v>1</v>
@@ -2013,28 +2004,28 @@
         <v>0.9999999997936998</v>
       </c>
       <c r="I23">
-        <v>0.99999999995963695</v>
+        <v>0.99999999993325583</v>
       </c>
       <c r="J23">
-        <v>0.9999999999936745</v>
+        <v>0.99999999998699796</v>
       </c>
       <c r="K23">
-        <v>0.99999999999836764</v>
+        <v>0.99999999999162092</v>
       </c>
       <c r="L23">
-        <v>0.99999999999977396</v>
+        <v>0.99999999999836775</v>
       </c>
       <c r="M23">
-        <v>0.99999999999973443</v>
+        <v>0.99999999999974709</v>
       </c>
       <c r="N23">
-        <v>0.99999999999978428</v>
+        <v>0.99999999999993849</v>
       </c>
       <c r="O23">
-        <v>0.99999999999996503</v>
+        <v>0.99999999999999012</v>
       </c>
       <c r="P23">
-        <v>0.99999999999999634</v>
+        <v>0.99999999999999034</v>
       </c>
       <c r="Q23">
         <v>1</v>
@@ -2051,22 +2042,22 @@
         <v>56</v>
       </c>
       <c r="H24">
-        <v>0.99999999999933187</v>
+        <v>0.99999999999950318</v>
       </c>
       <c r="I24">
-        <v>0.99999999999992728</v>
+        <v>0.99999999999981271</v>
       </c>
       <c r="J24">
-        <v>0.99999999999999145</v>
+        <v>0.99999999999998157</v>
       </c>
       <c r="K24">
-        <v>0.99999999999999845</v>
+        <v>0.9999999999999909</v>
       </c>
       <c r="L24">
-        <v>0.99999999999999989</v>
+        <v>0.99999999999999856</v>
       </c>
       <c r="M24">
-        <v>1</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="N24">
         <v>1</v>
@@ -2092,7 +2083,7 @@
         <v>58</v>
       </c>
       <c r="D25">
-        <v>0.99999998958979652</v>
+        <v>0.99999896939091004</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -2101,34 +2092,34 @@
         <v>1</v>
       </c>
       <c r="G25">
-        <v>0.99</v>
+        <v>0.5</v>
       </c>
       <c r="H25">
-        <v>0.99</v>
+        <v>0.5</v>
       </c>
       <c r="I25">
-        <v>0.99843918837795664</v>
+        <v>0.82291666666666663</v>
       </c>
       <c r="J25">
-        <v>0.99982193976085143</v>
+        <v>0.97917417309216692</v>
       </c>
       <c r="K25">
-        <v>0.99996215689272816</v>
+        <v>0.98626976920965403</v>
       </c>
       <c r="L25">
-        <v>0.99999520282787435</v>
+        <v>0.99768514192189284</v>
       </c>
       <c r="M25">
-        <v>0.99999550264978365</v>
+        <v>0.99956326456601607</v>
       </c>
       <c r="N25">
-        <v>0.99999645400895598</v>
+        <v>0.99992718425999116</v>
       </c>
       <c r="O25">
-        <v>0.99999963734067054</v>
+        <v>0.99999165116036937</v>
       </c>
       <c r="P25">
-        <v>0.99999991840162794</v>
+        <v>0.9999926333695609</v>
       </c>
       <c r="Q25">
         <v>1</v>
@@ -2145,28 +2136,28 @@
         <v>60</v>
       </c>
       <c r="H26">
-        <v>0.99999999998515776</v>
+        <v>0.99999999999630096</v>
       </c>
       <c r="I26">
-        <v>0.99999999999827638</v>
+        <v>0.99999999999859335</v>
       </c>
       <c r="J26">
-        <v>0.99999999999981237</v>
+        <v>0.99999999999988876</v>
       </c>
       <c r="K26">
-        <v>0.99999999999997535</v>
+        <v>0.99999999999995359</v>
       </c>
       <c r="L26">
-        <v>0.99999999999999833</v>
+        <v>0.99999999999999212</v>
       </c>
       <c r="M26">
         <v>0.99999999999999889</v>
       </c>
       <c r="N26">
-        <v>0.99999999999999922</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="O26">
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="P26">
         <v>1</v>
@@ -2185,44 +2176,41 @@
       <c r="C27" t="s">
         <v>62</v>
       </c>
-      <c r="D27">
-        <v>0.5</v>
-      </c>
       <c r="E27">
         <v>1</v>
       </c>
       <c r="F27">
-        <v>0.8</v>
+        <v>0.95454545454545459</v>
       </c>
       <c r="G27">
-        <v>0.8</v>
+        <v>0.95454545454545459</v>
       </c>
       <c r="H27">
-        <v>0.8</v>
+        <v>0.95454545454545459</v>
       </c>
       <c r="I27">
-        <v>0.95462184873949585</v>
+        <v>0.98286090969017792</v>
       </c>
       <c r="J27">
-        <v>0.99242443565871696</v>
+        <v>0.99582783984456325</v>
       </c>
       <c r="K27">
-        <v>0.99762802586431187</v>
+        <v>0.99707582785684323</v>
       </c>
       <c r="L27">
-        <v>0.99963988521815161</v>
+        <v>0.99927213524410508</v>
       </c>
       <c r="M27">
-        <v>0.99959079875145662</v>
+        <v>0.99980337203935765</v>
       </c>
       <c r="N27">
-        <v>0.99960784211716691</v>
+        <v>0.99995859821295774</v>
       </c>
       <c r="O27">
-        <v>0.99995612495519282</v>
+        <v>0.99998964923183431</v>
       </c>
       <c r="P27">
-        <v>0.99999021458448012</v>
+        <v>0.99998699163674165</v>
       </c>
       <c r="Q27">
         <v>1</v>
@@ -2239,43 +2227,43 @@
         <v>64</v>
       </c>
       <c r="D28">
-        <v>0.99999998958979652</v>
+        <v>0.99838644614764016</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>0.84</v>
       </c>
       <c r="G28">
-        <v>0.01</v>
+        <v>0.16000000000000003</v>
       </c>
       <c r="H28">
-        <v>0.01</v>
+        <v>0.16000000000000003</v>
       </c>
       <c r="I28">
-        <v>1.4996395097332376E-2</v>
+        <v>0.20936639118457304</v>
       </c>
       <c r="J28">
-        <v>2.682269022740336E-2</v>
+        <v>0.28163703149887853</v>
       </c>
       <c r="K28">
-        <v>3.167101871069352E-2</v>
+        <v>0.22330472434856574</v>
       </c>
       <c r="L28">
-        <v>5.1028409988000165E-2</v>
+        <v>0.32701898080216657</v>
       </c>
       <c r="M28">
-        <v>1.7852071732107302E-2</v>
+        <v>0.39751394132805745</v>
       </c>
       <c r="N28">
-        <v>6.1066691018100538E-3</v>
+        <v>0.51795944205656019</v>
       </c>
       <c r="O28">
-        <v>1.234954657430269E-2</v>
+        <v>0.66143725449776625</v>
       </c>
       <c r="P28">
-        <v>2.1555901594199109E-2</v>
+        <v>0.45364340652979923</v>
       </c>
       <c r="Q28">
         <v>1</v>
@@ -2292,7 +2280,7 @@
         <v>66</v>
       </c>
       <c r="D29">
-        <v>0.99999998958979652</v>
+        <v>0.99943914750420637</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -2307,28 +2295,28 @@
         <v>0.99</v>
       </c>
       <c r="I29">
-        <v>0.99808668776216058</v>
+        <v>0.99611901681759374</v>
       </c>
       <c r="J29">
-        <v>0.9996107649964876</v>
+        <v>0.99943702498983511</v>
       </c>
       <c r="K29">
-        <v>0.99</v>
+        <v>0.99977473390442462</v>
       </c>
       <c r="L29">
-        <v>0.99901365705614575</v>
+        <v>0.9999360628194639</v>
       </c>
       <c r="M29">
-        <v>0.99944083333544198</v>
+        <v>0.99998806851804778</v>
       </c>
       <c r="N29">
-        <v>0.99968306209426872</v>
+        <v>0.99999697624133754</v>
       </c>
       <c r="O29">
-        <v>0.99993424821364107</v>
+        <v>0.99999960250955444</v>
       </c>
       <c r="P29">
-        <v>0.99998343575813409</v>
+        <v>0.99999970188213616</v>
       </c>
       <c r="Q29">
         <v>1</v>
@@ -2345,28 +2333,28 @@
         <v>68</v>
       </c>
       <c r="H30">
-        <v>0.99999999998867484</v>
+        <v>0.99999999999303435</v>
       </c>
       <c r="I30">
-        <v>0.99999999999819111</v>
+        <v>0.99999999999771128</v>
       </c>
       <c r="J30">
-        <v>0.99999999999967348</v>
+        <v>0.99999999999969102</v>
       </c>
       <c r="K30">
-        <v>0.99999999999995537</v>
+        <v>0.999999999999859</v>
       </c>
       <c r="L30">
-        <v>0.99999999999999578</v>
+        <v>0.99999999999997158</v>
       </c>
       <c r="M30">
-        <v>0.99999999999999689</v>
+        <v>0.999999999999995</v>
       </c>
       <c r="N30">
-        <v>0.99999999999999778</v>
+        <v>0.99999999999999911</v>
       </c>
       <c r="O30">
-        <v>0.99999999999999978</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="P30">
         <v>1</v>
@@ -2385,44 +2373,41 @@
       <c r="C31" t="s">
         <v>70</v>
       </c>
-      <c r="D31">
-        <v>0.5</v>
-      </c>
       <c r="E31">
         <v>1</v>
       </c>
       <c r="F31">
-        <v>0.5</v>
+        <v>0.92</v>
       </c>
       <c r="G31">
-        <v>0.5</v>
+        <v>0.92</v>
       </c>
       <c r="H31">
-        <v>0.5</v>
+        <v>0.92</v>
       </c>
       <c r="I31">
-        <v>0.87283236994219648</v>
+        <v>0.97257142857142853</v>
       </c>
       <c r="J31">
-        <v>0.97777267508610799</v>
+        <v>0.99636358627529309</v>
       </c>
       <c r="K31">
-        <v>0.99611810894158315</v>
+        <v>0.99790307227502861</v>
       </c>
       <c r="L31">
-        <v>0.99970445146116249</v>
+        <v>0.99951531178950914</v>
       </c>
       <c r="M31">
-        <v>0.99972254124909965</v>
+        <v>0.99992136998093828</v>
       </c>
       <c r="N31">
-        <v>0.99976061470634447</v>
+        <v>0.99998938663749737</v>
       </c>
       <c r="O31">
-        <v>0.99998215366413501</v>
+        <v>0.99999881546176617</v>
       </c>
       <c r="P31">
-        <v>0.99999686478676597</v>
+        <v>0.99999890862759289</v>
       </c>
       <c r="Q31">
         <v>0</v>
@@ -2439,31 +2424,31 @@
         <v>72</v>
       </c>
       <c r="H32">
-        <v>0.99999999999917089</v>
+        <v>0.99999999999708433</v>
       </c>
       <c r="I32">
-        <v>0.99999999999987843</v>
+        <v>0.99999999999904143</v>
       </c>
       <c r="J32">
-        <v>0.99999999999998768</v>
+        <v>0.99999999999985212</v>
       </c>
       <c r="K32">
-        <v>0.99999999999999745</v>
+        <v>0.99999999999990408</v>
       </c>
       <c r="L32">
-        <v>0.99999999999999978</v>
+        <v>0.99999999999998013</v>
       </c>
       <c r="M32">
-        <v>0.99999999999999978</v>
+        <v>0.999999999999996</v>
       </c>
       <c r="N32">
-        <v>0.99999999999999978</v>
+        <v>0.99999999999999944</v>
       </c>
       <c r="O32">
-        <v>0.99</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="P32">
-        <v>0.9985304922850845</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="Q32">
         <v>1</v>
@@ -2480,7 +2465,7 @@
         <v>74</v>
       </c>
       <c r="D33">
-        <v>0.99999985276999992</v>
+        <v>0.99998542444029859</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -2495,28 +2480,28 @@
         <v>0.99</v>
       </c>
       <c r="I33">
-        <v>0.99869612956354659</v>
+        <v>0.99640546369518335</v>
       </c>
       <c r="J33">
-        <v>0.99980804086506891</v>
+        <v>0.99953878793469242</v>
       </c>
       <c r="K33">
-        <v>0.99998027477364881</v>
+        <v>0.99980667838312831</v>
       </c>
       <c r="L33">
-        <v>0.99999917235248459</v>
+        <v>0.99995290194974662</v>
       </c>
       <c r="M33">
-        <v>0.99999939097622348</v>
+        <v>0.99999563310675077</v>
       </c>
       <c r="N33">
-        <v>0.99999957921985694</v>
+        <v>0.99999932816778681</v>
       </c>
       <c r="O33">
-        <v>0.99999995820063214</v>
+        <v>0.99999998196422413</v>
       </c>
       <c r="P33">
-        <v>0.99999999157998309</v>
+        <v>0.9999999851705843</v>
       </c>
       <c r="Q33">
         <v>1</v>
@@ -2533,28 +2518,28 @@
         <v>0.99999998985050209</v>
       </c>
       <c r="I34">
-        <v>0.99999999836298414</v>
+        <v>0.99999999649380988</v>
       </c>
       <c r="J34">
-        <v>0.99999999969305942</v>
+        <v>0.99999999910859572</v>
       </c>
       <c r="K34">
-        <v>0.99999999994615074</v>
+        <v>0.99999999958935304</v>
       </c>
       <c r="L34">
-        <v>0.99999999999380496</v>
+        <v>0.99999999988671806</v>
       </c>
       <c r="M34">
-        <v>0.99999999999491695</v>
+        <v>0.99999999998459366</v>
       </c>
       <c r="N34">
-        <v>0.99999999999606071</v>
+        <v>0.99999999999516653</v>
       </c>
       <c r="O34">
-        <v>0.99999999999908318</v>
+        <v>0.99999999999932165</v>
       </c>
       <c r="P34">
-        <v>0.99999999999977862</v>
+        <v>0.99999999999938594</v>
       </c>
       <c r="Q34">
         <v>0</v>
@@ -2571,31 +2556,31 @@
         <v>78</v>
       </c>
       <c r="H35">
-        <v>0.89979431087889528</v>
+        <v>0.94906869462643306</v>
       </c>
       <c r="I35">
-        <v>0.8589120698484366</v>
+        <v>0.94280543659179195</v>
       </c>
       <c r="J35">
-        <v>0.79483142918388605</v>
+        <v>0.90817691515210019</v>
       </c>
       <c r="K35">
-        <v>0.64915828242331641</v>
+        <v>0.71747059916873523</v>
       </c>
       <c r="L35">
-        <v>0.51631796834745225</v>
+        <v>0.66388039086720996</v>
       </c>
       <c r="M35">
-        <v>0.2651577370884366</v>
+        <v>0.53074954729652779</v>
       </c>
       <c r="N35">
-        <v>9.8079502823927994E-2</v>
+        <v>0.50102356042318819</v>
       </c>
       <c r="O35">
-        <v>7.4183821104880074E-2</v>
+        <v>0.40548098332835752</v>
       </c>
       <c r="P35">
-        <v>6.1525710412094869E-2</v>
+        <v>0.17297717782287023</v>
       </c>
       <c r="Q35">
         <v>1</v>
@@ -2615,22 +2600,22 @@
         <v>0.99999999999622058</v>
       </c>
       <c r="I36">
-        <v>0.99999999999952438</v>
+        <v>0.99999999999892752</v>
       </c>
       <c r="J36">
-        <v>0.99999999999995071</v>
+        <v>0.99999999999989031</v>
       </c>
       <c r="K36">
-        <v>0.99999999999999256</v>
+        <v>0.99999999999994837</v>
       </c>
       <c r="L36">
+        <v>0.99999999999998979</v>
+      </c>
+      <c r="M36">
         <v>0.99999999999999911</v>
       </c>
-      <c r="M36">
-        <v>0.99999999999999922</v>
-      </c>
       <c r="N36">
-        <v>0.99999999999999944</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="O36">
         <v>1</v>
@@ -2653,34 +2638,34 @@
         <v>82</v>
       </c>
       <c r="H37">
-        <v>0.97281373279983541</v>
+        <v>0.99191215656213139</v>
       </c>
       <c r="I37">
-        <v>0.95782124487349074</v>
+        <v>0.99207931869145494</v>
       </c>
       <c r="J37">
-        <v>0.94377167509264326</v>
+        <v>0.9905102155414226</v>
       </c>
       <c r="K37">
-        <v>0.90885116954276413</v>
+        <v>0.96755548307615402</v>
       </c>
       <c r="L37">
-        <v>0.880454177591249</v>
+        <v>0.96788955444881075</v>
       </c>
       <c r="M37">
-        <v>0.68537414104594296</v>
+        <v>0.95169313051099236</v>
       </c>
       <c r="N37">
-        <v>0.36182779533135045</v>
+        <v>0.95414481930139694</v>
       </c>
       <c r="O37">
-        <v>0.32464208079301055</v>
+        <v>0.94516431791829469</v>
       </c>
       <c r="P37">
-        <v>0.2777473608677854</v>
+        <v>0.82959197402514229</v>
       </c>
       <c r="Q37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
@@ -2694,7 +2679,7 @@
         <v>84</v>
       </c>
       <c r="D38">
-        <v>0.99999998958979652</v>
+        <v>0.99999896939091004</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -2709,28 +2694,28 @@
         <v>0.99</v>
       </c>
       <c r="I38">
-        <v>0.99859254046446166</v>
+        <v>0.99650496295260726</v>
       </c>
       <c r="J38">
-        <v>0.99966732549265191</v>
+        <v>0.99948970490744138</v>
       </c>
       <c r="K38">
-        <v>0.99994453887335621</v>
+        <v>0.99972777779092858</v>
       </c>
       <c r="L38">
-        <v>0.99999475341375299</v>
+        <v>0.99993472774227765</v>
       </c>
       <c r="M38">
-        <v>0.99999594131525171</v>
+        <v>0.99998756653202769</v>
       </c>
       <c r="N38">
-        <v>0.99999712202014412</v>
+        <v>0.99999801062434723</v>
       </c>
       <c r="O38">
-        <v>0.99999967295600034</v>
+        <v>0.99999979059166377</v>
       </c>
       <c r="P38">
-        <v>0.99999990102613545</v>
+        <v>0.9999998332489104</v>
       </c>
       <c r="Q38">
         <v>1</v>
@@ -2747,31 +2732,31 @@
         <v>86</v>
       </c>
       <c r="H39">
-        <v>0.99999999965783559</v>
+        <v>0.99999999971609022</v>
       </c>
       <c r="I39">
-        <v>0.99999999994981592</v>
+        <v>0.99999999986863886</v>
       </c>
       <c r="J39">
-        <v>0.99999999999333222</v>
+        <v>0.99999999998190836</v>
       </c>
       <c r="K39">
-        <v>0.9999999999988487</v>
+        <v>0.99999999999086631</v>
       </c>
       <c r="L39">
-        <v>0.99999999999984879</v>
+        <v>0.99999999999764089</v>
       </c>
       <c r="M39">
-        <v>0.9999999999998852</v>
+        <v>0.99999999999963707</v>
       </c>
       <c r="N39">
-        <v>0.99999999999991662</v>
+        <v>0.99999999999992306</v>
       </c>
       <c r="O39">
-        <v>0.99999999999998912</v>
+        <v>0.99999999999998856</v>
       </c>
       <c r="P39">
-        <v>0.999999999999998</v>
+        <v>0.99999999999999156</v>
       </c>
       <c r="Q39">
         <v>1</v>
@@ -2788,28 +2773,28 @@
         <v>88</v>
       </c>
       <c r="H40">
-        <v>0.99999999999220635</v>
+        <v>0.99999999998994127</v>
       </c>
       <c r="I40">
-        <v>0.99999999999872768</v>
+        <v>0.99999999999612021</v>
       </c>
       <c r="J40">
-        <v>0.9999999999998298</v>
+        <v>0.99999999999956635</v>
       </c>
       <c r="K40">
-        <v>0.9999999999999718</v>
+        <v>0.99999999999976574</v>
       </c>
       <c r="L40">
-        <v>0.99999999999999689</v>
+        <v>0.99999999999995925</v>
       </c>
       <c r="M40">
-        <v>0.99999999999999722</v>
+        <v>0.99999999999999345</v>
       </c>
       <c r="N40">
-        <v>0.99999999999999778</v>
+        <v>0.99999999999999867</v>
       </c>
       <c r="O40">
-        <v>0.99999999999999978</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="P40">
         <v>1</v>
@@ -2829,31 +2814,31 @@
         <v>90</v>
       </c>
       <c r="H41">
-        <v>0.99999999983245358</v>
+        <v>0.99999999997299038</v>
       </c>
       <c r="I41">
-        <v>0.99999999997569933</v>
+        <v>0.99999999999052291</v>
       </c>
       <c r="J41">
-        <v>0.99999999999522293</v>
+        <v>0.99999999999886269</v>
       </c>
       <c r="K41">
-        <v>0.99999999999921041</v>
+        <v>0.99999999999941214</v>
       </c>
       <c r="L41">
-        <v>0.99999999999992883</v>
+        <v>0.99999999999989242</v>
       </c>
       <c r="M41">
-        <v>0.99999999999995415</v>
+        <v>0.99999999999997979</v>
       </c>
       <c r="N41">
-        <v>0.99999999999996769</v>
+        <v>0.99999999999999589</v>
       </c>
       <c r="O41">
-        <v>0.99999999999999467</v>
+        <v>0.99999999999999956</v>
       </c>
       <c r="P41">
-        <v>0.99999999999999867</v>
+        <v>0.99999999999999956</v>
       </c>
       <c r="Q41">
         <v>1</v>
@@ -2870,43 +2855,43 @@
         <v>92</v>
       </c>
       <c r="D42">
-        <v>0.99999998958979652</v>
+        <v>0.99990818106693591</v>
       </c>
       <c r="E42">
         <v>1</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="G42">
-        <v>0.8571428571428571</v>
+        <v>0.9375</v>
       </c>
       <c r="H42">
-        <v>0.8571428571428571</v>
+        <v>0.9375</v>
       </c>
       <c r="I42">
-        <v>0.97833523375142528</v>
+        <v>0.97762645914396884</v>
       </c>
       <c r="J42">
-        <v>0.99606727922317506</v>
+        <v>0.99697795880826456</v>
       </c>
       <c r="K42">
-        <v>0.99937226391510725</v>
+        <v>0.99857736202648917</v>
       </c>
       <c r="L42">
-        <v>0.99992209842447699</v>
+        <v>0.99957925342437803</v>
       </c>
       <c r="M42">
-        <v>0.99994756491183667</v>
+        <v>0.99992498952599607</v>
       </c>
       <c r="N42">
-        <v>0.99996758493289128</v>
+        <v>0.99998455574714684</v>
       </c>
       <c r="O42">
-        <v>0.99999569298190927</v>
+        <v>0.99999772645060014</v>
       </c>
       <c r="P42">
-        <v>0.9999989884999938</v>
+        <v>0.99999840367699988</v>
       </c>
       <c r="Q42">
         <v>1</v>
@@ -2923,31 +2908,31 @@
         <v>94</v>
       </c>
       <c r="H43">
-        <v>0.99999992963335127</v>
+        <v>0.99999999429517428</v>
       </c>
       <c r="I43">
-        <v>0.9999999861004143</v>
+        <v>0.99999999830397068</v>
       </c>
       <c r="J43">
-        <v>0.99999999740541068</v>
+        <v>0.99999999970503839</v>
       </c>
       <c r="K43">
-        <v>0.99999999928307404</v>
+        <v>0.99999999984002075</v>
       </c>
       <c r="L43">
-        <v>0.99999999987348365</v>
+        <v>0.99999999996739275</v>
       </c>
       <c r="M43">
-        <v>0.99999999987348365</v>
+        <v>0.99999999998983979</v>
       </c>
       <c r="N43">
-        <v>0.99999999989581012</v>
+        <v>0.99999999999713796</v>
       </c>
       <c r="O43">
-        <v>0.99999999996574584</v>
+        <v>0.99999999999950062</v>
       </c>
       <c r="P43">
-        <v>0.99999999999065803</v>
+        <v>0.99999999999945721</v>
       </c>
       <c r="Q43">
         <v>1</v>
@@ -2963,44 +2948,41 @@
       <c r="C44" t="s">
         <v>96</v>
       </c>
-      <c r="D44">
-        <v>0.5</v>
-      </c>
       <c r="E44">
         <v>0</v>
       </c>
       <c r="F44">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="G44">
-        <v>0.5</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="H44">
-        <v>0.5</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="I44">
-        <v>0.40697674418604651</v>
+        <v>0.16602316602316597</v>
       </c>
       <c r="J44">
-        <v>0.32056619483763532</v>
+        <v>9.449271442577499E-2</v>
       </c>
       <c r="K44">
-        <v>0.2111471569730152</v>
+        <v>2.8487116197337192E-2</v>
       </c>
       <c r="L44">
-        <v>0.15842405897573597</v>
+        <v>1.6580836404118483E-2</v>
       </c>
       <c r="M44">
-        <v>8.108567344837754E-2</v>
+        <v>1.0414715698970787E-2</v>
       </c>
       <c r="N44">
-        <v>2.6254558966805331E-2</v>
+        <v>8.0074176670128991E-3</v>
       </c>
       <c r="O44">
-        <v>2.1883492152902799E-2</v>
+        <v>4.7991233613438591E-3</v>
       </c>
       <c r="P44">
-        <v>1.5698754440870284E-2</v>
+        <v>1.9330677700535642E-3</v>
       </c>
       <c r="Q44">
         <v>1</v>
@@ -3016,44 +2998,41 @@
       <c r="C45" t="s">
         <v>98</v>
       </c>
-      <c r="D45">
-        <v>0.5</v>
-      </c>
       <c r="E45">
         <v>1</v>
       </c>
       <c r="F45">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="G45">
-        <v>0.99</v>
+        <v>0.875</v>
       </c>
       <c r="H45">
-        <v>0.99</v>
+        <v>0.875</v>
       </c>
       <c r="I45">
-        <v>0.99833139872315735</v>
+        <v>0.95454545454545459</v>
       </c>
       <c r="J45">
-        <v>0.99</v>
+        <v>0.99281867145421898</v>
       </c>
       <c r="K45">
-        <v>0.99795243345408724</v>
+        <v>0.99620745235612029</v>
       </c>
       <c r="L45">
-        <v>0.99979797279446658</v>
+        <v>0.99924918536612228</v>
       </c>
       <c r="M45">
-        <v>0.99980267017445601</v>
+        <v>0.99984608267583552</v>
       </c>
       <c r="N45">
-        <v>0.99983269360221705</v>
+        <v>0.99997191695425014</v>
       </c>
       <c r="O45">
-        <v>0.99998292535339572</v>
+        <v>0.99999581444604146</v>
       </c>
       <c r="P45">
-        <v>0.99999719483945815</v>
+        <v>0.99999591779263097</v>
       </c>
       <c r="Q45">
         <v>1</v>
@@ -3073,31 +3052,31 @@
         <v>0.9918196094976921</v>
       </c>
       <c r="I46">
-        <v>0.9912262959725302</v>
+        <v>0.9924691122896927</v>
       </c>
       <c r="J46">
-        <v>0.99100617458353801</v>
+        <v>0.98956090854928513</v>
       </c>
       <c r="K46">
-        <v>0.98804407594260557</v>
+        <v>0.98102671885452097</v>
       </c>
       <c r="L46">
-        <v>0.98675119677852585</v>
+        <v>0.98317911891292475</v>
       </c>
       <c r="M46">
-        <v>0.92368019460621675</v>
+        <v>0.98043050143313337</v>
       </c>
       <c r="N46">
-        <v>0.71549356333361203</v>
+        <v>0.97518244776678187</v>
       </c>
       <c r="O46">
-        <v>0.72497680785166485</v>
+        <v>0.97424043752213563</v>
       </c>
       <c r="P46">
-        <v>0.70347977956416008</v>
+        <v>0.01</v>
       </c>
       <c r="Q46">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
@@ -3111,31 +3090,31 @@
         <v>102</v>
       </c>
       <c r="H47">
-        <v>0.99999999999968248</v>
+        <v>0.99999999999926148</v>
       </c>
       <c r="I47">
-        <v>0.99999999999995826</v>
+        <v>0.99999999999970202</v>
       </c>
       <c r="J47">
-        <v>0.99999999999999589</v>
+        <v>0.9999999999999799</v>
       </c>
       <c r="K47">
-        <v>0.99999999999999967</v>
+        <v>0.99999999999999056</v>
       </c>
       <c r="L47">
-        <v>0.99</v>
+        <v>0.99999999999999833</v>
       </c>
       <c r="M47">
-        <v>0.99323882224645577</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="N47">
-        <v>0.99576352256265876</v>
+        <v>1</v>
       </c>
       <c r="O47">
-        <v>0.99957774559736545</v>
+        <v>1</v>
       </c>
       <c r="P47">
-        <v>0.99994141786449131</v>
+        <v>1</v>
       </c>
       <c r="Q47">
         <v>1</v>
@@ -3152,25 +3131,25 @@
         <v>104</v>
       </c>
       <c r="H48">
-        <v>0.99999999999928979</v>
+        <v>0.99999999999830813</v>
       </c>
       <c r="I48">
-        <v>0.99999999999990097</v>
+        <v>0.99999999999958789</v>
       </c>
       <c r="J48">
-        <v>0.99999999999998745</v>
+        <v>0.99999999999996669</v>
       </c>
       <c r="K48">
-        <v>0.99999999999999711</v>
+        <v>0.99999999999997868</v>
       </c>
       <c r="L48">
-        <v>0.99999999999999978</v>
+        <v>0.99999999999999678</v>
       </c>
       <c r="M48">
-        <v>0.99999999999999978</v>
+        <v>0.99999999999999944</v>
       </c>
       <c r="N48">
-        <v>0.99999999999999978</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="O48">
         <v>1</v>
@@ -3196,28 +3175,28 @@
         <v>0.99999957731875833</v>
       </c>
       <c r="I49">
-        <v>0.99999986488054782</v>
+        <v>0.99999981792188286</v>
       </c>
       <c r="J49">
-        <v>0.9999999639681425</v>
+        <v>0.99999991180590375</v>
       </c>
       <c r="K49">
-        <v>0.99999998352829333</v>
+        <v>0.99999993567018708</v>
       </c>
       <c r="L49">
-        <v>0.99999999529379813</v>
+        <v>0.99999997702506582</v>
       </c>
       <c r="M49">
-        <v>0.99999999104303516</v>
+        <v>0.99999999403013506</v>
       </c>
       <c r="N49">
-        <v>0.99999998857986983</v>
+        <v>0.9999999978875862</v>
       </c>
       <c r="O49">
-        <v>0.99999999705574771</v>
+        <v>0.99999999944504392</v>
       </c>
       <c r="P49">
-        <v>0.99999999921793303</v>
+        <v>0.99999999921801641</v>
       </c>
       <c r="Q49">
         <v>0</v>
@@ -3234,31 +3213,31 @@
         <v>108</v>
       </c>
       <c r="H50">
-        <v>0.99999999949071328</v>
+        <v>0.9999999975024878</v>
       </c>
       <c r="I50">
-        <v>0.99999999990247701</v>
+        <v>0.99999999919094673</v>
       </c>
       <c r="J50">
-        <v>0.99999999998338496</v>
+        <v>0.99999999986852894</v>
       </c>
       <c r="K50">
-        <v>0.99999999999774514</v>
+        <v>0.99999999992889843</v>
       </c>
       <c r="L50">
-        <v>0.99999999999980538</v>
+        <v>0.99999999998293565</v>
       </c>
       <c r="M50">
-        <v>0.99999999999985412</v>
+        <v>0.99999999999689015</v>
       </c>
       <c r="N50">
-        <v>0.99999999999990452</v>
+        <v>0.99999999999918965</v>
       </c>
       <c r="O50">
-        <v>0.99999999999998257</v>
+        <v>0.9999999999998983</v>
       </c>
       <c r="P50">
-        <v>0.99999999999999689</v>
+        <v>0.9999999999998983</v>
       </c>
       <c r="Q50">
         <v>1</v>
@@ -3275,7 +3254,7 @@
         <v>110</v>
       </c>
       <c r="D51">
-        <v>0.99999998958979652</v>
+        <v>0.9988789237668162</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -3290,28 +3269,28 @@
         <v>0.99</v>
       </c>
       <c r="I51">
-        <v>0.99744469591881435</v>
+        <v>0.99725274725274726</v>
       </c>
       <c r="J51">
-        <v>0.99957930164072362</v>
+        <v>0.99944933920704848</v>
       </c>
       <c r="K51">
-        <v>0.99989398918689709</v>
+        <v>0.99961686741217892</v>
       </c>
       <c r="L51">
-        <v>0.99998529642788314</v>
+        <v>0.99990543349875216</v>
       </c>
       <c r="M51">
-        <v>0.99998433751428606</v>
+        <v>0.9999816106683288</v>
       </c>
       <c r="N51">
-        <v>0.99998909214558573</v>
+        <v>0.99999570909544822</v>
       </c>
       <c r="O51">
-        <v>0.99999841076136853</v>
+        <v>0.99999925111306243</v>
       </c>
       <c r="P51">
-        <v>0.99</v>
+        <v>0.99999932600170582</v>
       </c>
       <c r="Q51">
         <v>1</v>
@@ -3328,31 +3307,31 @@
         <v>112</v>
       </c>
       <c r="H52">
-        <v>0.99999999906367976</v>
+        <v>0.99999999977948628</v>
       </c>
       <c r="I52">
-        <v>0.99999999972895992</v>
+        <v>0.99999999995966216</v>
       </c>
       <c r="J52">
-        <v>0.9999999999577599</v>
+        <v>0.99999999999495781</v>
       </c>
       <c r="K52">
-        <v>0.99999999998777256</v>
+        <v>0.99999999999645173</v>
       </c>
       <c r="L52">
-        <v>0.99999999999807854</v>
+        <v>0.99999999999935685</v>
       </c>
       <c r="M52">
-        <v>0.9999999999981587</v>
+        <v>0.9999999999998459</v>
       </c>
       <c r="N52">
-        <v>0.9999999999986362</v>
+        <v>0.99999999999997191</v>
       </c>
       <c r="O52">
-        <v>0.99999999999969313</v>
+        <v>0.99999999999999534</v>
       </c>
       <c r="P52">
-        <v>0.99999999999993638</v>
+        <v>0.99999999999999578</v>
       </c>
       <c r="Q52">
         <v>1</v>
@@ -3369,31 +3348,31 @@
         <v>114</v>
       </c>
       <c r="H53">
-        <v>0.99999999574647502</v>
+        <v>0.99999999780527171</v>
       </c>
       <c r="I53">
-        <v>0.99999999909612591</v>
+        <v>0.99999999959356889</v>
       </c>
       <c r="J53">
-        <v>0.99999999984332844</v>
+        <v>0.99999999994123878</v>
       </c>
       <c r="K53">
-        <v>0.99999999995670918</v>
+        <v>0.9999999999615381</v>
       </c>
       <c r="L53">
-        <v>0.99999999999081701</v>
+        <v>0.99999999999221023</v>
       </c>
       <c r="M53">
-        <v>0.99999999999061739</v>
+        <v>0.99999999999817024</v>
       </c>
       <c r="N53">
-        <v>0.99999999999260203</v>
+        <v>0.99999999999958245</v>
       </c>
       <c r="O53">
-        <v>0.999999999998198</v>
+        <v>0.99999999999991762</v>
       </c>
       <c r="P53">
-        <v>0.99999999999964839</v>
+        <v>0.99999999999992106</v>
       </c>
       <c r="Q53">
         <v>1</v>
@@ -3410,7 +3389,7 @@
         <v>116</v>
       </c>
       <c r="D54">
-        <v>0.99999998958979652</v>
+        <v>0.99949520444220097</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -3425,28 +3404,28 @@
         <v>0.99</v>
       </c>
       <c r="I54">
-        <v>0.99840764331210197</v>
+        <v>0.99618320610687017</v>
       </c>
       <c r="J54">
-        <v>0.99975763451284527</v>
+        <v>0.99944460684010528</v>
       </c>
       <c r="K54">
-        <v>0.99996344529973891</v>
+        <v>0.99973404329775106</v>
       </c>
       <c r="L54">
-        <v>0.99999665333179721</v>
+        <v>0.99994679733986691</v>
       </c>
       <c r="M54">
-        <v>0.99999762014475491</v>
+        <v>0.9999925180338356</v>
       </c>
       <c r="N54">
-        <v>0.999998430306971</v>
+        <v>0.99999863963418789</v>
       </c>
       <c r="O54">
-        <v>0.99999980522030529</v>
+        <v>0.99999985528005686</v>
       </c>
       <c r="P54">
-        <v>0.99999996431516469</v>
+        <v>0.99999986794305018</v>
       </c>
       <c r="Q54">
         <v>1</v>
@@ -3463,31 +3442,31 @@
         <v>118</v>
       </c>
       <c r="H55">
-        <v>0.99999734955792507</v>
+        <v>0.99999923628065579</v>
       </c>
       <c r="I55">
-        <v>0.9999989704877732</v>
+        <v>0.99999959936019844</v>
       </c>
       <c r="J55">
-        <v>0.99999959001700078</v>
+        <v>0.99999980937295752</v>
       </c>
       <c r="K55">
-        <v>0.9999997891515584</v>
+        <v>0.99999982626395834</v>
       </c>
       <c r="L55">
-        <v>0.9999999240185693</v>
+        <v>0.99999992339197419</v>
       </c>
       <c r="M55">
-        <v>0.99999990063966993</v>
+        <v>0.99999995885865123</v>
       </c>
       <c r="N55">
-        <v>0.99999990063966993</v>
+        <v>0.99999998586747529</v>
       </c>
       <c r="O55">
-        <v>0.99999996792304091</v>
+        <v>0.99999999478060164</v>
       </c>
       <c r="P55">
-        <v>0.99999998690190806</v>
+        <v>0.99999999284196794</v>
       </c>
       <c r="Q55">
         <v>1</v>
@@ -3504,22 +3483,22 @@
         <v>120</v>
       </c>
       <c r="H56">
-        <v>0.99999999999978162</v>
+        <v>0.99999999999978695</v>
       </c>
       <c r="I56">
-        <v>0.99999999999997236</v>
+        <v>0.99999999999993383</v>
       </c>
       <c r="J56">
-        <v>0.99999999999999611</v>
+        <v>0.99999999999999389</v>
       </c>
       <c r="K56">
+        <v>0.999999999999996</v>
+      </c>
+      <c r="L56">
         <v>0.99999999999999933</v>
       </c>
-      <c r="L56">
-        <v>1</v>
-      </c>
       <c r="M56">
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="N56">
         <v>1</v>
@@ -3545,31 +3524,31 @@
         <v>122</v>
       </c>
       <c r="H57">
-        <v>0.99999999873842671</v>
+        <v>0.99999999865245082</v>
       </c>
       <c r="I57">
-        <v>0.99999999973845433</v>
+        <v>0.99999999958675156</v>
       </c>
       <c r="J57">
-        <v>0.99999999993909217</v>
+        <v>0.9999999999376229</v>
       </c>
       <c r="K57">
-        <v>0.99999999998458033</v>
+        <v>0.99999999995292288</v>
       </c>
       <c r="L57">
-        <v>0.99999999999735667</v>
+        <v>0.99999999999002342</v>
       </c>
       <c r="M57">
-        <v>0.99999999999762101</v>
+        <v>0.99999999999750588</v>
       </c>
       <c r="N57">
-        <v>0.99999999999785893</v>
+        <v>0.99999999999946676</v>
       </c>
       <c r="O57">
-        <v>0.99999999999955602</v>
+        <v>0.99999999999989408</v>
       </c>
       <c r="P57">
-        <v>0.99999999999988898</v>
+        <v>0.99999999999991007</v>
       </c>
       <c r="Q57">
         <v>1</v>
@@ -3586,31 +3565,31 @@
         <v>124</v>
       </c>
       <c r="H58">
-        <v>0.99999995769278693</v>
+        <v>0.99999997226842086</v>
       </c>
       <c r="I58">
-        <v>0.99999999206739731</v>
+        <v>0.99999998570090431</v>
       </c>
       <c r="J58">
-        <v>0.99999999825723118</v>
+        <v>0.99999999618037849</v>
       </c>
       <c r="K58">
-        <v>0.99999999950206597</v>
+        <v>0.99999999735564671</v>
       </c>
       <c r="L58">
-        <v>0.99999999991257649</v>
+        <v>0.99999999909938686</v>
       </c>
       <c r="M58">
-        <v>0.99999999990286281</v>
+        <v>0.99999999977484677</v>
       </c>
       <c r="N58">
-        <v>0.99999999990691024</v>
+        <v>0.99999999993682753</v>
       </c>
       <c r="O58">
-        <v>0.99999999998098876</v>
+        <v>0.99999999998396139</v>
       </c>
       <c r="P58">
-        <v>0.99999999999514311</v>
+        <v>0.9999999999855832</v>
       </c>
       <c r="Q58">
         <v>1</v>
@@ -3627,31 +3606,31 @@
         <v>126</v>
       </c>
       <c r="H59">
-        <v>0.99999999999923406</v>
+        <v>0.99999999999586819</v>
       </c>
       <c r="I59">
-        <v>0.99999999999990219</v>
+        <v>0.99999999999860156</v>
       </c>
       <c r="J59">
-        <v>0.99999999999998668</v>
+        <v>0.99999999999982303</v>
       </c>
       <c r="K59">
-        <v>0.99999999999999867</v>
+        <v>0.99999999999991596</v>
       </c>
       <c r="L59">
-        <v>1</v>
+        <v>0.9999999999999849</v>
       </c>
       <c r="M59">
-        <v>1</v>
+        <v>0.999999999999998</v>
       </c>
       <c r="N59">
-        <v>1</v>
+        <v>0.99999999999999956</v>
       </c>
       <c r="O59">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="P59">
-        <v>1</v>
+        <v>0.99037138927097657</v>
       </c>
       <c r="Q59">
         <v>1</v>
@@ -3668,31 +3647,31 @@
         <v>128</v>
       </c>
       <c r="H60">
-        <v>0.99999999997968847</v>
+        <v>0.9999999990139874</v>
       </c>
       <c r="I60">
-        <v>0.99999999999684352</v>
+        <v>0.99999999961416897</v>
       </c>
       <c r="J60">
-        <v>0.99999999999955225</v>
+        <v>0.99999999993650879</v>
       </c>
       <c r="K60">
-        <v>0.99999999999992961</v>
+        <v>0.99999999996947531</v>
       </c>
       <c r="L60">
-        <v>0.99999999999999512</v>
+        <v>0.99999999999308098</v>
       </c>
       <c r="M60">
-        <v>0.99999999999999623</v>
+        <v>0.99</v>
       </c>
       <c r="N60">
-        <v>0.99999999999999745</v>
+        <v>0.99760411528433512</v>
       </c>
       <c r="O60">
-        <v>0.99999999999999967</v>
+        <v>0.99968439125803565</v>
       </c>
       <c r="P60">
-        <v>1</v>
+        <v>0.99972946602361812</v>
       </c>
       <c r="Q60">
         <v>1</v>
@@ -3708,44 +3687,41 @@
       <c r="C61" t="s">
         <v>130</v>
       </c>
-      <c r="D61">
-        <v>0.5</v>
-      </c>
       <c r="E61">
         <v>1</v>
       </c>
       <c r="F61">
-        <v>1</v>
+        <v>0.91304347826086951</v>
       </c>
       <c r="G61">
-        <v>0.99</v>
+        <v>0.91304347826086951</v>
       </c>
       <c r="H61">
-        <v>0.99</v>
+        <v>0.91304347826086951</v>
       </c>
       <c r="I61">
-        <v>0.99708454810495628</v>
+        <v>0.96963946869070206</v>
       </c>
       <c r="J61">
-        <v>0.99935953886798501</v>
+        <v>0.99530659657850895</v>
       </c>
       <c r="K61">
-        <v>0.99982524738417189</v>
+        <v>0.9966926352820964</v>
       </c>
       <c r="L61">
-        <v>0.99997538325957036</v>
+        <v>0.99940632888532877</v>
       </c>
       <c r="M61">
-        <v>0.99997485951230325</v>
+        <v>0.99985954113734288</v>
       </c>
       <c r="N61">
-        <v>0.99997969412330268</v>
+        <v>0.99996464269247953</v>
       </c>
       <c r="O61">
-        <v>0.9999947932863319</v>
+        <v>0.99999363550012044</v>
       </c>
       <c r="P61">
-        <v>0.99999859818714021</v>
+        <v>0.99999322925819789</v>
       </c>
       <c r="Q61">
         <v>1</v>
@@ -3762,31 +3738,31 @@
         <v>132</v>
       </c>
       <c r="H62">
-        <v>9.0242275468779831E-2</v>
+        <v>0.24835692793333164</v>
       </c>
       <c r="I62">
-        <v>3.6927846495510862E-2</v>
+        <v>0.19152980309493614</v>
       </c>
       <c r="J62">
-        <v>1.5924106844971565E-2</v>
+        <v>8.7463557597503391E-2</v>
       </c>
       <c r="K62">
-        <v>5.3649907388220452E-3</v>
+        <v>1.9857939538876726E-2</v>
       </c>
       <c r="L62">
-        <v>2.3352953231384642E-3</v>
+        <v>1.0945404553334582E-2</v>
       </c>
       <c r="M62">
-        <v>9.2801168205423055E-4</v>
+        <v>4.3090459334654474E-3</v>
       </c>
       <c r="N62">
-        <v>3.0952872486648183E-4</v>
+        <v>2.7572920373399082E-3</v>
       </c>
       <c r="O62">
-        <v>1.6338626414103222E-4</v>
+        <v>1.2092091972651328E-3</v>
       </c>
       <c r="P62">
-        <v>9.9941629169533188E-5</v>
+        <v>5.2010640614239174E-4</v>
       </c>
       <c r="Q62">
         <v>1</v>
@@ -3800,31 +3776,31 @@
         <v>134</v>
       </c>
       <c r="H63">
-        <v>0.99999999983487364</v>
+        <v>0.99999999979402654</v>
       </c>
       <c r="I63">
-        <v>0.99999999997113176</v>
+        <v>0.99999999994711497</v>
       </c>
       <c r="J63">
-        <v>0.99999999999674727</v>
+        <v>0.99999999999357825</v>
       </c>
       <c r="K63">
-        <v>0.99999999999955858</v>
+        <v>0.999999999996527</v>
       </c>
       <c r="L63">
-        <v>0.99999999999995126</v>
+        <v>0.99999999999949296</v>
       </c>
       <c r="M63">
-        <v>0.99999999999995925</v>
+        <v>0.99999999999991118</v>
       </c>
       <c r="N63">
-        <v>0.9999999999999688</v>
+        <v>0.99999999999997968</v>
       </c>
       <c r="O63">
-        <v>0.999999999999994</v>
+        <v>0.99999999999999678</v>
       </c>
       <c r="P63">
-        <v>0.99999999999999845</v>
+        <v>0.99999999999999711</v>
       </c>
       <c r="Q63">
         <v>0</v>
@@ -3844,28 +3820,28 @@
         <v>0.99999999994765099</v>
       </c>
       <c r="I64">
-        <v>0.99999999999018463</v>
+        <v>0.99999999998740974</v>
       </c>
       <c r="J64">
-        <v>0.99999999999828049</v>
+        <v>0.99999999999795053</v>
       </c>
       <c r="K64">
-        <v>0.99999999999971545</v>
+        <v>0.99999999999879563</v>
       </c>
       <c r="L64">
-        <v>0.99999999999996469</v>
+        <v>0.99999999999975331</v>
       </c>
       <c r="M64">
-        <v>0.9999999999999708</v>
+        <v>0.99999999999995937</v>
       </c>
       <c r="N64">
-        <v>0.99999999999997968</v>
+        <v>0.9999999999999909</v>
       </c>
       <c r="O64">
-        <v>0.99999999999999722</v>
+        <v>0.99999999999999878</v>
       </c>
       <c r="P64">
-        <v>0.99999999999999967</v>
+        <v>0.99999999999999889</v>
       </c>
       <c r="Q64">
         <v>1</v>
@@ -3882,31 +3858,31 @@
         <v>138</v>
       </c>
       <c r="H65">
-        <v>0.99999971534939158</v>
+        <v>0.99999973018917832</v>
       </c>
       <c r="I65">
-        <v>0.99999990383423576</v>
+        <v>0.99999986301910304</v>
       </c>
       <c r="J65">
-        <v>0.99999997073215674</v>
+        <v>0.99999996371366606</v>
       </c>
       <c r="K65">
-        <v>0.99999999212019586</v>
+        <v>0.99999998096454579</v>
       </c>
       <c r="L65">
-        <v>0.99999999864917644</v>
+        <v>0.99999999361047687</v>
       </c>
       <c r="M65">
-        <v>0.99999999897437475</v>
+        <v>0.99999999797741712</v>
       </c>
       <c r="N65">
-        <v>0.99999999918724047</v>
+        <v>0.99999999936433115</v>
       </c>
       <c r="O65">
-        <v>0.99999999969521514</v>
+        <v>0.9999999998377016</v>
       </c>
       <c r="P65">
-        <v>0.99999999988147259</v>
+        <v>0.9999999998377016</v>
       </c>
       <c r="Q65">
         <v>1</v>
@@ -3923,31 +3899,31 @@
         <v>140</v>
       </c>
       <c r="H66">
-        <v>0.99999999612367518</v>
+        <v>0.99999999008591811</v>
       </c>
       <c r="I66">
-        <v>0.99999999940563022</v>
+        <v>0.99999999622985614</v>
       </c>
       <c r="J66">
-        <v>0.99999999986593169</v>
+        <v>0.99999999906970471</v>
       </c>
       <c r="K66">
-        <v>0.99999999997588707</v>
+        <v>0.99999999950749074</v>
       </c>
       <c r="L66">
-        <v>0.99999999999743472</v>
+        <v>0.99999999987039223</v>
       </c>
       <c r="M66">
-        <v>0.99999999999759182</v>
+        <v>0.99999999997830102</v>
       </c>
       <c r="N66">
-        <v>0.99999999999817168</v>
+        <v>0.99999999999382183</v>
       </c>
       <c r="O66">
-        <v>0.99999999999966194</v>
+        <v>0.99999999999908884</v>
       </c>
       <c r="P66">
-        <v>0.99999999999992684</v>
+        <v>0.99999999999903399</v>
       </c>
       <c r="Q66">
         <v>1</v>
@@ -3964,31 +3940,31 @@
         <v>142</v>
       </c>
       <c r="H67">
-        <v>0.99318177630525151</v>
+        <v>0.99166113395102107</v>
       </c>
       <c r="I67">
-        <v>0.99443076999133562</v>
+        <v>0.9918732133834306</v>
       </c>
       <c r="J67">
-        <v>0.99550881229297972</v>
+        <v>0.99072301416453923</v>
       </c>
       <c r="K67">
-        <v>0.99493224100909095</v>
+        <v>0.98549875246881491</v>
       </c>
       <c r="L67">
-        <v>0.99533256684755012</v>
+        <v>0.98532450326734633</v>
       </c>
       <c r="M67">
-        <v>0.98452037150350835</v>
+        <v>0.98532450326734633</v>
       </c>
       <c r="N67">
-        <v>0.94607743744455275</v>
+        <v>0.98532450326734633</v>
       </c>
       <c r="O67">
-        <v>0.95099470456961277</v>
+        <v>0.98634929376914904</v>
       </c>
       <c r="P67">
-        <v>0.9566967160135279</v>
+        <v>0.95976112366860733</v>
       </c>
       <c r="Q67">
         <v>0</v>
@@ -4005,31 +3981,31 @@
         <v>144</v>
       </c>
       <c r="H68">
-        <v>0.99999999836288367</v>
+        <v>0.99999999328917866</v>
       </c>
       <c r="I68">
-        <v>0.99999999965654895</v>
+        <v>0.99999999816977603</v>
       </c>
       <c r="J68">
-        <v>0.99999999994920796</v>
+        <v>0.99999999951836216</v>
       </c>
       <c r="K68">
-        <v>0.99999999998621925</v>
+        <v>0.99999999969897624</v>
       </c>
       <c r="L68">
-        <v>0.99999999999808875</v>
+        <v>0.99999999992572153</v>
       </c>
       <c r="M68">
-        <v>0.99999999999796407</v>
+        <v>0.99999999998345446</v>
       </c>
       <c r="N68">
-        <v>0.99999999999824363</v>
+        <v>0.99999999999543576</v>
       </c>
       <c r="O68">
-        <v>0.99999999999968925</v>
+        <v>0.99999999999902034</v>
       </c>
       <c r="P68">
-        <v>0.99999999999994049</v>
+        <v>0.99999999999893674</v>
       </c>
       <c r="Q68">
         <v>1</v>
@@ -4046,31 +4022,31 @@
         <v>146</v>
       </c>
       <c r="H69">
-        <v>0.9999999995141563</v>
+        <v>0.99999999829662611</v>
       </c>
       <c r="I69">
-        <v>0.99</v>
+        <v>0.9999999993762293</v>
       </c>
       <c r="J69">
-        <v>0.99833139872315735</v>
+        <v>0.99999999986867982</v>
       </c>
       <c r="K69">
-        <v>0.99968290245008229</v>
+        <v>0.99999999992777389</v>
       </c>
       <c r="L69">
-        <v>0.9999583260697229</v>
+        <v>0.99999999997919886</v>
       </c>
       <c r="M69">
-        <v>0.99996332675795807</v>
+        <v>0.99999999999642808</v>
       </c>
       <c r="N69">
-        <v>0.99996907924549971</v>
+        <v>0.99999999999898792</v>
       </c>
       <c r="O69">
-        <v>0.99999546483634316</v>
+        <v>0.99999999999982869</v>
       </c>
       <c r="P69">
-        <v>0.99999884977343989</v>
+        <v>0.99999999999984046</v>
       </c>
       <c r="Q69">
         <v>1</v>
@@ -4087,31 +4063,31 @@
         <v>148</v>
       </c>
       <c r="H70">
-        <v>0.99999999866197087</v>
+        <v>0.99999999941453854</v>
       </c>
       <c r="I70">
-        <v>0.99999999973892117</v>
+        <v>0.99999999980751952</v>
       </c>
       <c r="J70">
-        <v>0.99999999996318112</v>
+        <v>0.99999999997873767</v>
       </c>
       <c r="K70">
-        <v>0.99999999999281586</v>
+        <v>0.99999999998919453</v>
       </c>
       <c r="L70">
-        <v>0.99999999999932043</v>
+        <v>0.99999999999806577</v>
       </c>
       <c r="M70">
-        <v>0.99999999999942701</v>
+        <v>0.99999999999954259</v>
       </c>
       <c r="N70">
-        <v>0.99999999999962819</v>
+        <v>0.99999999999989642</v>
       </c>
       <c r="O70">
-        <v>0.9999999999999164</v>
+        <v>0.9999999999999829</v>
       </c>
       <c r="P70">
-        <v>0.99999999999998013</v>
+        <v>0.99999999999998368</v>
       </c>
       <c r="Q70">
         <v>1</v>
@@ -4128,31 +4104,31 @@
         <v>150</v>
       </c>
       <c r="H71">
-        <v>0.9999999999815844</v>
+        <v>0.99999999960431629</v>
       </c>
       <c r="I71">
-        <v>0.99999999999715539</v>
+        <v>0.99999999985161858</v>
       </c>
       <c r="J71">
-        <v>0.99999999999973932</v>
+        <v>0.99999999997414557</v>
       </c>
       <c r="K71">
-        <v>0.99999999999996902</v>
+        <v>0.99999999998883571</v>
       </c>
       <c r="L71">
-        <v>0.99999999999999734</v>
+        <v>0.9999999999974305</v>
       </c>
       <c r="M71">
-        <v>0.999999999999998</v>
+        <v>0.9999999999996273</v>
       </c>
       <c r="N71">
-        <v>0.999999999999999</v>
+        <v>0.99999999999990918</v>
       </c>
       <c r="O71">
-        <v>0.99999999999999989</v>
+        <v>0.99999999999998945</v>
       </c>
       <c r="P71">
-        <v>1</v>
+        <v>0.99999999999999156</v>
       </c>
       <c r="Q71">
         <v>1</v>
@@ -4165,11 +4141,41 @@
       <c r="C72" t="s">
         <v>152</v>
       </c>
-      <c r="D72">
-        <v>0.5</v>
-      </c>
       <c r="E72">
         <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0.8</v>
+      </c>
+      <c r="G72">
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="H72">
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="I72">
+        <v>0.29251700680272102</v>
+      </c>
+      <c r="J72">
+        <v>0.32211304601614937</v>
+      </c>
+      <c r="K72">
+        <v>0.26823633194009783</v>
+      </c>
+      <c r="L72">
+        <v>0.37924276169265025</v>
+      </c>
+      <c r="M72">
+        <v>0.48637621762670125</v>
+      </c>
+      <c r="N72">
+        <v>0.57800494844482275</v>
+      </c>
+      <c r="O72">
+        <v>0.67616069290822989</v>
+      </c>
+      <c r="P72">
+        <v>0.44081225067225144</v>
       </c>
       <c r="Q72">
         <v>0</v>
@@ -4186,31 +4192,31 @@
         <v>154</v>
       </c>
       <c r="H73">
-        <v>0.99999999999897282</v>
+        <v>0.99999999998540745</v>
       </c>
       <c r="I73">
-        <v>0.99999999999984934</v>
+        <v>0.99999999999520239</v>
       </c>
       <c r="J73">
-        <v>0.99999999999997868</v>
+        <v>0.99999999999927747</v>
       </c>
       <c r="K73">
-        <v>0.99999999999999656</v>
+        <v>0.99999999999962463</v>
       </c>
       <c r="L73">
+        <v>0.99999999999992162</v>
+      </c>
+      <c r="M73">
+        <v>0.99999999999998679</v>
+      </c>
+      <c r="N73">
+        <v>0.99999999999999745</v>
+      </c>
+      <c r="O73">
         <v>0.99999999999999978</v>
       </c>
-      <c r="M73">
+      <c r="P73">
         <v>0.99999999999999978</v>
-      </c>
-      <c r="N73">
-        <v>0.99999999999999978</v>
-      </c>
-      <c r="O73">
-        <v>1</v>
-      </c>
-      <c r="P73">
-        <v>1</v>
       </c>
       <c r="Q73">
         <v>1</v>
@@ -4224,31 +4230,31 @@
         <v>156</v>
       </c>
       <c r="H74">
-        <v>0.99999999714491117</v>
+        <v>0.99999999854405408</v>
       </c>
       <c r="I74">
-        <v>0.99999999935220674</v>
+        <v>0.9999999996234622</v>
       </c>
       <c r="J74">
-        <v>0.99999999987498733</v>
+        <v>0.99999999992247757</v>
       </c>
       <c r="K74">
-        <v>0.9999999999693151</v>
+        <v>0.999999999959436</v>
       </c>
       <c r="L74">
-        <v>0.99999999999436984</v>
+        <v>0.99999999999128619</v>
       </c>
       <c r="M74">
-        <v>0.9999999999956366</v>
+        <v>0.99999999999776201</v>
       </c>
       <c r="N74">
-        <v>0.9999999999972603</v>
+        <v>0.99999999999951428</v>
       </c>
       <c r="O74">
-        <v>0.9999999999994611</v>
+        <v>0.99999999999989264</v>
       </c>
       <c r="P74">
-        <v>0.9999999999998731</v>
+        <v>0.99999999999990652</v>
       </c>
       <c r="Q74">
         <v>0</v>
@@ -4265,31 +4271,31 @@
         <v>158</v>
       </c>
       <c r="H75">
-        <v>0.99999977016312203</v>
+        <v>0.99999984836703892</v>
       </c>
       <c r="I75">
-        <v>0.99999991583437042</v>
+        <v>0.9999999719198186</v>
       </c>
       <c r="J75">
-        <v>0.99999997194478851</v>
+        <v>0.99999999186642996</v>
       </c>
       <c r="K75">
-        <v>0.99999999025860697</v>
+        <v>0.99999999362072944</v>
       </c>
       <c r="L75">
-        <v>0.99999999717185362</v>
+        <v>0.9999999981522113</v>
       </c>
       <c r="M75">
-        <v>0.99999999634410341</v>
+        <v>0.99999999936091521</v>
       </c>
       <c r="N75">
-        <v>0.999999996855929</v>
+        <v>0.9999999998114929</v>
       </c>
       <c r="O75">
-        <v>0.9999999988486501</v>
+        <v>0.99999999993570299</v>
       </c>
       <c r="P75">
-        <v>0.9999999996859954</v>
+        <v>0.99999999993296695</v>
       </c>
       <c r="Q75">
         <v>0</v>
@@ -4306,31 +4312,31 @@
         <v>160</v>
       </c>
       <c r="H76">
-        <v>0.99999999941128692</v>
+        <v>0.99999999941839746</v>
       </c>
       <c r="I76">
-        <v>0.99999999985068866</v>
+        <v>0.99999999975555831</v>
       </c>
       <c r="J76">
-        <v>0.99999999997035727</v>
+        <v>0.9999999999376914</v>
       </c>
       <c r="K76">
-        <v>0.99999999999224731</v>
+        <v>0.99999999995999123</v>
       </c>
       <c r="L76">
-        <v>0.99999999999892475</v>
+        <v>0.99999999998913669</v>
       </c>
       <c r="M76">
-        <v>0.99999999999890188</v>
+        <v>0.9999999999970568</v>
       </c>
       <c r="N76">
-        <v>0.99999999999896916</v>
+        <v>0.99999999999936096</v>
       </c>
       <c r="O76">
-        <v>0.99999999999985756</v>
+        <v>0.99999999999988121</v>
       </c>
       <c r="P76">
-        <v>0.99999999999996902</v>
+        <v>0.99999999999985145</v>
       </c>
       <c r="Q76">
         <v>1</v>
@@ -4347,31 +4353,31 @@
         <v>162</v>
       </c>
       <c r="H77">
-        <v>0.99999999932272932</v>
+        <v>0.99999999981727805</v>
       </c>
       <c r="I77">
-        <v>0.99999999984519528</v>
+        <v>0.99999999992691124</v>
       </c>
       <c r="J77">
-        <v>0.99999999997307754</v>
+        <v>0.99999999998612232</v>
       </c>
       <c r="K77">
-        <v>0.99999999999160016</v>
+        <v>0.99999999999059908</v>
       </c>
       <c r="L77">
-        <v>0.9999999999986835</v>
+        <v>0.99999999999807154</v>
       </c>
       <c r="M77">
-        <v>0.99999999999871081</v>
+        <v>0.99999999999954847</v>
       </c>
       <c r="N77">
-        <v>0.99999999999893396</v>
+        <v>0.99999999999992761</v>
       </c>
       <c r="O77">
-        <v>0.99999999999985967</v>
+        <v>0.99999999999998546</v>
       </c>
       <c r="P77">
-        <v>0.99999999999997058</v>
+        <v>0.99999999999998168</v>
       </c>
       <c r="Q77">
         <v>1</v>
@@ -4388,31 +4394,31 @@
         <v>164</v>
       </c>
       <c r="H78">
-        <v>0.94170945201433642</v>
+        <v>0.87646539350049857</v>
       </c>
       <c r="I78">
-        <v>0.92156500361491511</v>
+        <v>0.89128719524273881</v>
       </c>
       <c r="J78">
-        <v>0.88574286505526056</v>
+        <v>0.84475700425229694</v>
       </c>
       <c r="K78">
-        <v>0.7949178311514139</v>
+        <v>0.67824699338157357</v>
       </c>
       <c r="L78">
-        <v>0.74906137407780826</v>
+        <v>0.63993955595241092</v>
       </c>
       <c r="M78">
-        <v>0.41417098889444853</v>
+        <v>0.54148982849789218</v>
       </c>
       <c r="N78">
-        <v>0.16900632330997542</v>
+        <v>0.51669684222255996</v>
       </c>
       <c r="O78">
-        <v>0.14280621820101436</v>
+        <v>0.42194313777010201</v>
       </c>
       <c r="P78">
-        <v>0.11896721523402846</v>
+        <v>0.18830800290249006</v>
       </c>
       <c r="Q78">
         <v>1</v>
@@ -4429,28 +4435,28 @@
         <v>0.9999999999708703</v>
       </c>
       <c r="I79">
-        <v>0.99999999999450839</v>
+        <v>0.99999999999196421</v>
       </c>
       <c r="J79">
-        <v>0.99999999999903655</v>
+        <v>0.99999999999844469</v>
       </c>
       <c r="K79">
-        <v>0.99999999999978684</v>
+        <v>0.9999999999991086</v>
       </c>
       <c r="L79">
-        <v>0.99999999999997358</v>
+        <v>0.99999999999984435</v>
       </c>
       <c r="M79">
-        <v>0.99999999999997435</v>
+        <v>0.99999999999997324</v>
       </c>
       <c r="N79">
-        <v>0.99999999999998113</v>
+        <v>0.99999999999999689</v>
       </c>
       <c r="O79">
-        <v>0.99999999999999745</v>
+        <v>0.99999999999999967</v>
       </c>
       <c r="P79">
-        <v>0.99999999999999944</v>
+        <v>0.99999999999999967</v>
       </c>
       <c r="Q79">
         <v>0</v>
@@ -4467,31 +4473,31 @@
         <v>168</v>
       </c>
       <c r="H80">
-        <v>0.99999999999335587</v>
+        <v>0.99999999999344247</v>
       </c>
       <c r="I80">
-        <v>0.999999999999032</v>
+        <v>0.99999999999821154</v>
       </c>
       <c r="J80">
-        <v>0.99999999999989464</v>
+        <v>0.99999999999977518</v>
       </c>
       <c r="K80">
-        <v>0.99999999999997635</v>
+        <v>0.99999999999986322</v>
       </c>
       <c r="L80">
-        <v>0.99999999999999778</v>
+        <v>0.99999999999997702</v>
       </c>
       <c r="M80">
-        <v>0.99999999999999811</v>
+        <v>0.99999999999999567</v>
       </c>
       <c r="N80">
-        <v>0.99999999999999867</v>
+        <v>0.99999999999999933</v>
       </c>
       <c r="O80">
         <v>0.99999999999999989</v>
       </c>
       <c r="P80">
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="Q80">
         <v>1</v>
@@ -4508,31 +4514,31 @@
         <v>170</v>
       </c>
       <c r="H81">
-        <v>0.99879079324593956</v>
+        <v>0.99857308427989866</v>
       </c>
       <c r="I81">
-        <v>0.99870349404037584</v>
+        <v>0.99851371782486942</v>
       </c>
       <c r="J81">
-        <v>0.99867112446376161</v>
+        <v>0.99822381071724631</v>
       </c>
       <c r="K81">
-        <v>0.99804817392025236</v>
+        <v>0.9945513264758894</v>
       </c>
       <c r="L81">
-        <v>0.99807314911514899</v>
+        <v>0.99471895221255491</v>
       </c>
       <c r="M81">
-        <v>0.99363479048612113</v>
+        <v>0.9937321587561202</v>
       </c>
       <c r="N81">
-        <v>0.98034071962976965</v>
+        <v>0.99412569699055364</v>
       </c>
       <c r="O81">
-        <v>0.98286102490632687</v>
+        <v>0.99417279434730965</v>
       </c>
       <c r="P81">
-        <v>0.98417295835908558</v>
+        <v>0.9778917196151371</v>
       </c>
       <c r="Q81">
         <v>0</v>
@@ -4549,31 +4555,31 @@
         <v>172</v>
       </c>
       <c r="H82">
-        <v>0.99999999935190242</v>
+        <v>0.99999999841017073</v>
       </c>
       <c r="I82">
-        <v>0.99999999979260878</v>
+        <v>0.99999999959235153</v>
       </c>
       <c r="J82">
-        <v>0.99999999995515876</v>
+        <v>0.99999999993040145</v>
       </c>
       <c r="K82">
-        <v>0.99999999998231603</v>
+        <v>0.99999999994268352</v>
       </c>
       <c r="L82">
-        <v>0.99999999999571287</v>
+        <v>0.99</v>
       </c>
       <c r="M82">
-        <v>0.99999999999503086</v>
+        <v>0.99771566783122811</v>
       </c>
       <c r="N82">
-        <v>0.99999999999533518</v>
+        <v>0.99950317093842245</v>
       </c>
       <c r="O82">
-        <v>0.99999999999896338</v>
+        <v>0.99991112675589999</v>
       </c>
       <c r="P82">
-        <v>0.99999999999972444</v>
+        <v>0.99989953575822388</v>
       </c>
       <c r="Q82">
         <v>1</v>
@@ -4590,43 +4596,43 @@
         <v>174</v>
       </c>
       <c r="D83">
-        <v>0.99999896939091004</v>
+        <v>0.99996599102162964</v>
       </c>
       <c r="E83">
         <v>1</v>
       </c>
       <c r="F83">
-        <v>1</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="G83">
-        <v>0.99</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="H83">
-        <v>0.99</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="I83">
-        <v>0.99597585513078468</v>
+        <v>0.98266253869969045</v>
       </c>
       <c r="J83">
-        <v>0.99859396014182666</v>
+        <v>0.99697839785712905</v>
       </c>
       <c r="K83">
-        <v>0.99954355343649692</v>
+        <v>0.99777478083490689</v>
       </c>
       <c r="L83">
-        <v>0.99987871572672393</v>
+        <v>0.99958461079224714</v>
       </c>
       <c r="M83">
-        <v>0.99989326828613168</v>
+        <v>0.99990858475542765</v>
       </c>
       <c r="N83">
-        <v>0.99993375004723062</v>
+        <v>0.99997211982066236</v>
       </c>
       <c r="O83">
-        <v>0.99997607539330291</v>
+        <v>0.9999931279804416</v>
       </c>
       <c r="P83">
-        <v>0.99999008823833213</v>
+        <v>0.99999205900811017</v>
       </c>
       <c r="Q83">
         <v>1</v>
@@ -4646,25 +4652,25 @@
         <v>0.99999999999550593</v>
       </c>
       <c r="I84">
-        <v>0.99999999999925626</v>
+        <v>0.99999999999902045</v>
       </c>
       <c r="J84">
-        <v>0.99999999999989297</v>
+        <v>0.99999999999984845</v>
       </c>
       <c r="K84">
-        <v>0.99999999999998013</v>
+        <v>0.99999999999990996</v>
       </c>
       <c r="L84">
-        <v>0.99999999999999845</v>
+        <v>0.99999999999998224</v>
       </c>
       <c r="M84">
-        <v>0.99999999999999845</v>
+        <v>0.99999999999999778</v>
       </c>
       <c r="N84">
-        <v>0.99999999999999856</v>
+        <v>0.99999999999999967</v>
       </c>
       <c r="O84">
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
       <c r="P84">
         <v>1</v>
@@ -4684,31 +4690,31 @@
         <v>178</v>
       </c>
       <c r="H85">
-        <v>0.99999999994835798</v>
+        <v>0.99999999910117365</v>
       </c>
       <c r="I85">
-        <v>0.99999999999433609</v>
+        <v>0.99999999969218267</v>
       </c>
       <c r="J85">
-        <v>0.99999999999937927</v>
+        <v>0.99999999995264355</v>
       </c>
       <c r="K85">
-        <v>0.99999999999988753</v>
+        <v>0.99999999997492883</v>
       </c>
       <c r="L85">
-        <v>0.99999999999998701</v>
+        <v>0.99999999999538158</v>
       </c>
       <c r="M85">
-        <v>0.99999999999998923</v>
+        <v>0.9999999999993614</v>
       </c>
       <c r="N85">
-        <v>0.99999999999999278</v>
+        <v>0.99999999999985512</v>
       </c>
       <c r="O85">
-        <v>0.999999999999999</v>
+        <v>0.99999999999997302</v>
       </c>
       <c r="P85">
-        <v>0.99999999999999989</v>
+        <v>0.99999999999997879</v>
       </c>
       <c r="Q85">
         <v>1</v>
@@ -4725,22 +4731,22 @@
         <v>0.99999999999561873</v>
       </c>
       <c r="I86">
-        <v>0.99999999999942701</v>
+        <v>0.99999999999848654</v>
       </c>
       <c r="J86">
-        <v>0.99999999999991263</v>
+        <v>0.99999999999973577</v>
       </c>
       <c r="K86">
-        <v>0.99999999999998501</v>
+        <v>0.99999999999986167</v>
       </c>
       <c r="L86">
-        <v>0.99999999999999922</v>
+        <v>0.99999999999997324</v>
       </c>
       <c r="M86">
+        <v>0.99999999999999722</v>
+      </c>
+      <c r="N86">
         <v>0.99999999999999944</v>
-      </c>
-      <c r="N86">
-        <v>0.99999999999999967</v>
       </c>
       <c r="O86">
         <v>1</v>
@@ -4763,31 +4769,31 @@
         <v>182</v>
       </c>
       <c r="H87">
-        <v>0.45093261006628621</v>
+        <v>0.46593432221757858</v>
       </c>
       <c r="I87">
-        <v>0.298266926212788</v>
+        <v>0.39552263429632645</v>
       </c>
       <c r="J87">
-        <v>0.18603960784348098</v>
+        <v>0.23353095580211744</v>
       </c>
       <c r="K87">
-        <v>7.9554672603901463E-2</v>
+        <v>8.3750046650583027E-2</v>
       </c>
       <c r="L87">
-        <v>4.3755267119910526E-2</v>
+        <v>5.3094974006647901E-2</v>
       </c>
       <c r="M87">
-        <v>1.5231695136319024E-2</v>
+        <v>2.8206849118149989E-2</v>
       </c>
       <c r="N87">
-        <v>6.1039363809135532E-3</v>
+        <v>2.0274590125371375E-2</v>
       </c>
       <c r="O87">
-        <v>4.2567151698146774E-3</v>
+        <v>1.0800465191167712E-2</v>
       </c>
       <c r="P87">
-        <v>3.0802706809370541E-3</v>
+        <v>4.4914666490213952E-3</v>
       </c>
       <c r="Q87">
         <v>1</v>
@@ -4804,31 +4810,31 @@
         <v>184</v>
       </c>
       <c r="H88">
-        <v>0.99845979673578167</v>
+        <v>0.99836557140098159</v>
       </c>
       <c r="I88">
-        <v>0.99803081897061818</v>
+        <v>0.99880284066729441</v>
       </c>
       <c r="J88">
-        <v>0.99789372361783535</v>
+        <v>0.99858042952670567</v>
       </c>
       <c r="K88">
-        <v>0.99694879125587299</v>
+        <v>0.99575334543098992</v>
       </c>
       <c r="L88">
-        <v>0.99618889618816009</v>
+        <v>0.99609865864894387</v>
       </c>
       <c r="M88">
-        <v>0.97194337338325743</v>
+        <v>0.99554380775980089</v>
       </c>
       <c r="N88">
-        <v>0.89770893514061456</v>
+        <v>0.99646706939611174</v>
       </c>
       <c r="O88">
-        <v>0.91504239079730609</v>
+        <v>0.99666268829129057</v>
       </c>
       <c r="P88">
-        <v>0.93596807768417145</v>
+        <v>0.98871354283662616</v>
       </c>
       <c r="Q88">
         <v>0</v>
@@ -4845,10 +4851,10 @@
         <v>186</v>
       </c>
       <c r="H89">
-        <v>1</v>
+        <v>0.99999999999999911</v>
       </c>
       <c r="I89">
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="J89">
         <v>1</v>
@@ -4883,28 +4889,28 @@
         <v>188</v>
       </c>
       <c r="H90">
-        <v>0.99999999999804046</v>
+        <v>0.99999999998700762</v>
       </c>
       <c r="I90">
-        <v>0.99999999999976941</v>
+        <v>0.99999999999618883</v>
       </c>
       <c r="J90">
-        <v>0.9999999999999728</v>
+        <v>0.99999999999939215</v>
       </c>
       <c r="K90">
-        <v>0.999999999999995</v>
+        <v>0.9999999999996465</v>
       </c>
       <c r="L90">
-        <v>0.99999999999999956</v>
+        <v>0.9999999999999436</v>
       </c>
       <c r="M90">
-        <v>0.99999999999999956</v>
+        <v>0.99999999999999067</v>
       </c>
       <c r="N90">
-        <v>0.99999999999999956</v>
+        <v>0.99999999999999878</v>
       </c>
       <c r="O90">
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="P90">
         <v>1</v>
@@ -4924,25 +4930,25 @@
         <v>190</v>
       </c>
       <c r="H91">
-        <v>0.99999999999464495</v>
+        <v>0.99999999997445577</v>
       </c>
       <c r="I91">
-        <v>0.99999999999916211</v>
+        <v>0.99999999999037459</v>
       </c>
       <c r="J91">
-        <v>0.99999999999990108</v>
+        <v>0.99999999999926825</v>
       </c>
       <c r="K91">
-        <v>0.99999999999998435</v>
+        <v>0.99999999999968536</v>
       </c>
       <c r="L91">
+        <v>0.99999999999995726</v>
+      </c>
+      <c r="M91">
+        <v>0.99999999999999489</v>
+      </c>
+      <c r="N91">
         <v>0.99999999999999889</v>
-      </c>
-      <c r="M91">
-        <v>0.99999999999999922</v>
-      </c>
-      <c r="N91">
-        <v>0.99999999999999944</v>
       </c>
       <c r="O91">
         <v>0.99999999999999989</v>
@@ -4965,31 +4971,31 @@
         <v>192</v>
       </c>
       <c r="H92">
-        <v>0.99999999996117617</v>
+        <v>0.99999999998780142</v>
       </c>
       <c r="I92">
-        <v>0.99999999999565614</v>
+        <v>0.99999999999551525</v>
       </c>
       <c r="J92">
-        <v>0.99999999999929279</v>
+        <v>0.99999999999938338</v>
       </c>
       <c r="K92">
-        <v>0.99999999999989364</v>
+        <v>0.99999999999971967</v>
       </c>
       <c r="L92">
-        <v>0.99999999999998745</v>
+        <v>0.99999999999994904</v>
       </c>
       <c r="M92">
-        <v>0.99999999999998856</v>
+        <v>0.99999999999999223</v>
       </c>
       <c r="N92">
-        <v>0.99999999999999045</v>
+        <v>0.99999999999999867</v>
       </c>
       <c r="O92">
-        <v>0.99999999999999878</v>
+        <v>0.99999999999999989</v>
       </c>
       <c r="P92">
-        <v>0.99999999999999978</v>
+        <v>1</v>
       </c>
       <c r="Q92">
         <v>1</v>
@@ -5006,31 +5012,31 @@
         <v>194</v>
       </c>
       <c r="H93">
-        <v>0.96868386516196359</v>
+        <v>0.97499650968701146</v>
       </c>
       <c r="I93">
-        <v>0.96307275516020796</v>
+        <v>0.97446683420767577</v>
       </c>
       <c r="J93">
-        <v>0.9567315698657276</v>
+        <v>0.9616708268220574</v>
       </c>
       <c r="K93">
-        <v>0.92608947055898816</v>
+        <v>0.88569229765177004</v>
       </c>
       <c r="L93">
-        <v>0.88676472056695921</v>
+        <v>0.86755183599794439</v>
       </c>
       <c r="M93">
-        <v>0.49466779701573516</v>
+        <v>0.79665831936246845</v>
       </c>
       <c r="N93">
-        <v>0.01</v>
+        <v>0.78511756335067784</v>
       </c>
       <c r="O93">
-        <v>8.8105726872246722E-3</v>
+        <v>0.74818356822345755</v>
       </c>
       <c r="P93">
-        <v>6.1523899668717479E-3</v>
+        <v>0.38171654418832268</v>
       </c>
       <c r="Q93">
         <v>1</v>
@@ -5047,31 +5053,31 @@
         <v>196</v>
       </c>
       <c r="H94">
-        <v>0.99999999989185617</v>
+        <v>0.99999999986947896</v>
       </c>
       <c r="I94">
-        <v>0.99999999998272704</v>
+        <v>0.99999999995081812</v>
       </c>
       <c r="J94">
-        <v>0.99999999999790257</v>
+        <v>0.99999999999337941</v>
       </c>
       <c r="K94">
-        <v>0.99999999999967848</v>
+        <v>0.99999999999688438</v>
       </c>
       <c r="L94">
-        <v>0.99999999999997458</v>
+        <v>0.99999999999936418</v>
       </c>
       <c r="M94">
-        <v>0.99999999999997813</v>
+        <v>0.99999999999991762</v>
       </c>
       <c r="N94">
-        <v>0.99999999999998201</v>
+        <v>0.99999999999998379</v>
       </c>
       <c r="O94">
-        <v>0.99999999999999745</v>
+        <v>0.99999999999999878</v>
       </c>
       <c r="P94">
-        <v>0.99999999999999944</v>
+        <v>0.999999999999999</v>
       </c>
       <c r="Q94">
         <v>1</v>
@@ -5088,43 +5094,43 @@
         <v>198</v>
       </c>
       <c r="D95">
-        <v>0.99999998958979652</v>
+        <v>0.99497487437185939</v>
       </c>
       <c r="E95">
         <v>0</v>
       </c>
       <c r="F95">
-        <v>1</v>
+        <v>0.89655172413793105</v>
       </c>
       <c r="G95">
-        <v>0.01</v>
+        <v>0.10344827586206895</v>
       </c>
       <c r="H95">
-        <v>0.01</v>
+        <v>0.10344827586206895</v>
       </c>
       <c r="I95">
-        <v>4.2723631508678238E-3</v>
+        <v>7.5313807531380728E-2</v>
       </c>
       <c r="J95">
-        <v>1.7054186703683511E-3</v>
+        <v>2.8765481422293234E-2</v>
       </c>
       <c r="K95">
-        <v>5.4460227603359771E-4</v>
+        <v>6.6198103955540984E-3</v>
       </c>
       <c r="L95">
-        <v>2.3193291008422176E-4</v>
+        <v>3.4891670464777596E-3</v>
       </c>
       <c r="M95">
-        <v>1.0987637001160309E-4</v>
+        <v>1.2893485144293464E-3</v>
       </c>
       <c r="N95">
-        <v>4.3953445671677179E-5</v>
+        <v>7.2058678542507595E-4</v>
       </c>
       <c r="O95">
-        <v>2.3221169718254753E-5</v>
+        <v>2.8672145110661613E-4</v>
       </c>
       <c r="P95">
-        <v>1.2605911663744783E-5</v>
+        <v>1.4204145916493709E-4</v>
       </c>
       <c r="Q95">
         <v>1</v>
@@ -5141,31 +5147,31 @@
         <v>200</v>
       </c>
       <c r="H96">
-        <v>1.0388216395741752E-2</v>
+        <v>6.8871263032420863E-3</v>
       </c>
       <c r="I96">
-        <v>4.181348610813802E-3</v>
+        <v>4.4466766240258545E-3</v>
       </c>
       <c r="J96">
-        <v>1.4213347961188291E-3</v>
+        <v>1.5290428613924188E-3</v>
       </c>
       <c r="K96">
-        <v>4.2113649712509821E-4</v>
+        <v>3.1842653031756657E-4</v>
       </c>
       <c r="L96">
-        <v>1.5180179156316773E-4</v>
+        <v>1.5671141705037969E-4</v>
       </c>
       <c r="M96">
-        <v>6.4406389241956788E-5</v>
+        <v>6.5523742929629426E-5</v>
       </c>
       <c r="N96">
-        <v>2.4270048341690351E-5</v>
+        <v>3.1688783967339389E-5</v>
       </c>
       <c r="O96">
-        <v>1.1185472985841166E-5</v>
+        <v>1.1215922826529538E-5</v>
       </c>
       <c r="P96">
-        <v>5.6926380563361809E-6</v>
+        <v>4.4298483206314684E-6</v>
       </c>
       <c r="Q96">
         <v>1</v>
@@ -5182,43 +5188,43 @@
         <v>202</v>
       </c>
       <c r="D97">
-        <v>0.99999998958979652</v>
+        <v>0.99999896939091004</v>
       </c>
       <c r="E97">
         <v>0</v>
       </c>
       <c r="F97">
-        <v>1</v>
+        <v>0.81481481481481477</v>
       </c>
       <c r="G97">
-        <v>0.01</v>
+        <v>0.18518518518518523</v>
       </c>
       <c r="H97">
-        <v>0.01</v>
+        <v>0.18518518518518523</v>
       </c>
       <c r="I97">
-        <v>4.1076368513706081E-3</v>
+        <v>0.12178619756427611</v>
       </c>
       <c r="J97">
-        <v>1.4784291582436427E-3</v>
+        <v>5.070697220867873E-2</v>
       </c>
       <c r="K97">
-        <v>4.9329592146383735E-4</v>
+        <v>1.0405452457087523E-2</v>
       </c>
       <c r="L97">
-        <v>2.0752021809588385E-4</v>
+        <v>5.4413783534578812E-3</v>
       </c>
       <c r="M97">
-        <v>1.0042376486527894E-4</v>
+        <v>2.26936088246525E-3</v>
       </c>
       <c r="N97">
-        <v>4.1716936115235348E-5</v>
+        <v>1.1936616123318759E-3</v>
       </c>
       <c r="O97">
-        <v>1.9952012404761352E-5</v>
+        <v>4.8055154551853487E-4</v>
       </c>
       <c r="P97">
-        <v>1.0883014556252299E-5</v>
+        <v>2.0952798542959232E-4</v>
       </c>
       <c r="Q97">
         <v>1</v>
@@ -5235,34 +5241,34 @@
         <v>204</v>
       </c>
       <c r="H98">
-        <v>0.99032795734264045</v>
+        <v>0.99651215078638311</v>
       </c>
       <c r="I98">
-        <v>0.98902351947861378</v>
+        <v>0.99747855489563109</v>
       </c>
       <c r="J98">
-        <v>0.98876511088385566</v>
+        <v>0.99693341234509003</v>
       </c>
       <c r="K98">
-        <v>0.9803426093162384</v>
+        <v>0.9923080529151852</v>
       </c>
       <c r="L98">
-        <v>0.9711057999110202</v>
+        <v>0.9923080529151852</v>
       </c>
       <c r="M98">
-        <v>0.01</v>
+        <v>0.9907838415388639</v>
       </c>
       <c r="N98">
-        <v>1.2610340479192945E-3</v>
+        <v>0.99203495488056026</v>
       </c>
       <c r="O98">
-        <v>1.2085544637696394E-3</v>
+        <v>0.99203495488056026</v>
       </c>
       <c r="P98">
-        <v>1.2872717719690009E-3</v>
+        <v>0.95291711904703391</v>
       </c>
       <c r="Q98">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
@@ -5276,31 +5282,31 @@
         <v>206</v>
       </c>
       <c r="H99">
-        <v>0.38130514384647723</v>
+        <v>0.43205672291729114</v>
       </c>
       <c r="I99">
-        <v>0.24665460994622668</v>
+        <v>0.40693539449240401</v>
       </c>
       <c r="J99">
-        <v>0.13065223412141719</v>
+        <v>0.21411120979081122</v>
       </c>
       <c r="K99">
-        <v>5.670616601560622E-2</v>
+        <v>5.816235897332897E-2</v>
       </c>
       <c r="L99">
-        <v>2.4686743388611675E-2</v>
+        <v>3.4770686548091567E-2</v>
       </c>
       <c r="M99">
-        <v>9.5852011612131954E-3</v>
+        <v>1.4204617194438702E-2</v>
       </c>
       <c r="N99">
-        <v>2.4457551083534694E-3</v>
+        <v>9.0517810830254425E-3</v>
       </c>
       <c r="O99">
-        <v>1.4215738913305983E-3</v>
+        <v>4.6624999051509955E-3</v>
       </c>
       <c r="P99">
-        <v>8.488451835968017E-4</v>
+        <v>1.8035584049633738E-3</v>
       </c>
       <c r="Q99">
         <v>1</v>
@@ -5317,31 +5323,31 @@
         <v>208</v>
       </c>
       <c r="H100">
-        <v>0.35031449562914591</v>
+        <v>0.24243954809858143</v>
       </c>
       <c r="I100">
-        <v>0.19249728466737209</v>
+        <v>0.20636285481752767</v>
       </c>
       <c r="J100">
-        <v>8.9255762243946782E-2</v>
+        <v>9.6061315803098971E-2</v>
       </c>
       <c r="K100">
-        <v>3.1327849572873066E-2</v>
+        <v>1.922625795934586E-2</v>
       </c>
       <c r="L100">
-        <v>1.3357271088270957E-2</v>
+        <v>1.1399812336597618E-2</v>
       </c>
       <c r="M100">
-        <v>4.9971031260247758E-3</v>
+        <v>4.4817562894717599E-3</v>
       </c>
       <c r="N100">
-        <v>1.6451980984786927E-3</v>
+        <v>2.2676664718897584E-3</v>
       </c>
       <c r="O100">
-        <v>8.781131652398302E-4</v>
+        <v>1.0259245365271407E-3</v>
       </c>
       <c r="P100">
-        <v>5.8205464052755746E-4</v>
+        <v>4.1273831288221472E-4</v>
       </c>
       <c r="Q100">
         <v>1</v>
@@ -5358,31 +5364,31 @@
         <v>210</v>
       </c>
       <c r="H101">
-        <v>0.89107345080658695</v>
+        <v>0.62648745012684115</v>
       </c>
       <c r="I101">
-        <v>0.86266479296680065</v>
+        <v>0.65030073296550084</v>
       </c>
       <c r="J101">
-        <v>0.83049509121765308</v>
+        <v>0.52371642729407164</v>
       </c>
       <c r="K101">
-        <v>0.69390397293134132</v>
+        <v>0.30224686392547501</v>
       </c>
       <c r="L101">
-        <v>0.57145903480164872</v>
+        <v>0.24344710200196892</v>
       </c>
       <c r="M101">
-        <v>6.9694476020231627E-2</v>
+        <v>0.14689089317132667</v>
       </c>
       <c r="N101">
-        <v>9.8309771302717112E-3</v>
+        <v>0.11571652779977473</v>
       </c>
       <c r="O101">
-        <v>7.7025581942383493E-3</v>
+        <v>8.3914663507618739E-2</v>
       </c>
       <c r="P101">
-        <v>6.9670876369046257E-3</v>
+        <v>1.3978239952936709E-2</v>
       </c>
       <c r="Q101">
         <v>1</v>
@@ -5393,34 +5399,34 @@
         <v>211</v>
       </c>
       <c r="H102">
+        <v>79.569892473118273</v>
+      </c>
+      <c r="I102">
         <v>80.645161290322577</v>
-      </c>
-      <c r="I102">
-        <v>81.72043010752688</v>
       </c>
       <c r="J102">
         <v>81.72043010752688</v>
       </c>
       <c r="K102">
-        <v>80.645161290322577</v>
+        <v>83.870967741935488</v>
       </c>
       <c r="L102">
-        <v>82.79569892473117</v>
+        <v>83.870967741935488</v>
       </c>
       <c r="M102">
-        <v>88.172043010752688</v>
+        <v>84.946236559139791</v>
       </c>
       <c r="N102">
-        <v>90.322580645161281</v>
+        <v>83.870967741935488</v>
       </c>
       <c r="O102">
-        <v>90.322580645161281</v>
+        <v>86.021505376344081</v>
       </c>
       <c r="P102">
-        <v>90.322580645161281</v>
+        <v>89.247311827956992</v>
       </c>
       <c r="Q102">
-        <v>90.322580645161281</v>
+        <v>89.247311827956992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>